<commit_message>
EE-1836 Edited the readme within the whole_submission_template.xlsx      to add a wider description.
</commit_message>
<xml_diff>
--- a/templates/sequence-based-metadata/whole_submission_template.xlsx
+++ b/templates/sequence-based-metadata/whole_submission_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcasado\Documents\GitHub\ega-metadata-schema\templates\sequence-based-metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcasado\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415ACAE5-4F4C-4541-8A42-173C0D8D1AAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B603BEAF-F063-4D25-BE2A-6EB53080DA39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8490" yWindow="5475" windowWidth="19425" windowHeight="11625" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="405">
   <si>
     <t>Tag</t>
   </si>
@@ -556,58 +556,9 @@
     <t>Column headers</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Descriptive</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> row (explains what type of data corresponds to each column)</t>
-    </r>
-  </si>
-  <si>
-    <t>Real data ceiling (put your real data beneath this row)</t>
-  </si>
-  <si>
     <t>4 onwards</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Real data</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (all rows from 4 onwards will be transformed into XMLs)</t>
-    </r>
-  </si>
-  <si>
     <t>Column headers' colour format</t>
   </si>
   <si>
@@ -623,13 +574,7 @@
     <t>No colour</t>
   </si>
   <si>
-    <t>Optional (highly recommended) attributes</t>
-  </si>
-  <si>
     <t>Other colours</t>
-  </si>
-  <si>
-    <t>Repeated blocks (each with their own colour): you can add or remove as many "whole" blocks as you want to fulfil your needs, but remember to always work with complete repetitions (e.g. TAG-VALUE-UNITS columns for an attribute)</t>
   </si>
   <si>
     <t>Platform*</t>
@@ -711,32 +656,6 @@
   </si>
   <si>
     <t>Columns related to a choice from another column (based on multiple choice attributes) - e.g. if the provided experiment's layout is PAIRED, the two related columns (PAIRED.Nominal_length and PAIRED.Nominal_sdev) will change their header's format to light yellow.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Column headers that do not appear to be chosen for any metadata instance (row), and thus </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>can be ignored</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (based on multiple choice attributes)</t>
-    </r>
   </si>
   <si>
     <t>Study_alias*</t>
@@ -1701,12 +1620,267 @@
   <si>
     <t>9ddd9749fdc4118a2c614140cea6c7c3</t>
   </si>
+  <si>
+    <t>Optional ( yet highly recommended) attributes</t>
+  </si>
+  <si>
+    <t>Repeated blocks (each with their own colour): you can add or remove as many "whole" blocks as you want to fulfil your needs, but remember to always work with complete repetitions (e.g. adding three new columns TAG-VALUE-UNITS for a new attribute, but not adding only one or two of them TAG-VALUE)</t>
+  </si>
+  <si>
+    <t>Real data "ceiling" (put your real data beneath this row)</t>
+  </si>
+  <si>
+    <t>What is metadata?</t>
+  </si>
+  <si>
+    <t>What is this file?</t>
+  </si>
+  <si>
+    <t>This is a template spreadsheet (.xlsx) of metadata.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For what? </t>
+  </si>
+  <si>
+    <t>What are these tabs?</t>
+  </si>
+  <si>
+    <t>Each excel tab besides this one (Readme) represents a metadata object within the data model of the EGA. In other words, each tab will hold the information of one single metadata object (e.g. sample, study…)</t>
+  </si>
+  <si>
+    <t>You simply have to fill out the rows and columns of the tabs that are relevant to your submission (i.e. if you are only submitting samples' metadata, other tabs can be left empty). In each tab you will find a grey line at the third row, below which you shall enter your real metadata. In the begining, the template will contain a "mock" example at row 4 for you to visualise (contains things like "Example!_..."), remove it and use your real metadata there.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ok, but </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>what do I do</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">? </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Metadata is simply data (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>units of information</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) that describe other data. For instance, if we think about data being a sequence of nucleotides, its metadata could be the genomic coordinates of such sequence, or its associated phenotype. </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Repeated columns? </t>
+  </si>
+  <si>
+    <t>Read this overview before anything else!</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descriptive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> row (explains what type of data corresponds to each column). Fields that do not start with "TODO:…" must contain the string that is left within this row. For instance, one of the TAG columns within the Sample tab is "phenotype", which means that this column shall contain "phenotype" for each and every row. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Real data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (all rows from 4 onwards will be transformed into XML nodes by the star2xml tool)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Column headers that do not appear to be chosen for any metadata instance (row), and thus </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>can be ignored</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (i.e. left empty) (based on multiple choice attributes)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Within each tab, you will find a dark vertical line, beyond which there will be repeated "blocks" of columns. These blocks can be repeated indefinetely (i.e. add or remove as many of this blocks/columns as you need) but always as a complete block. See the column headers' format below. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This template shall be filled with the metadata associated to your datafiles, and then used as input of the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>star2xml</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tool (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://github.com/EbiEga/ega-metadata-schema/tree/main/Star2xml</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>), which will create XMLs with such metadata. These files then can be used during a programmatic metadata submission to the European Genome-phenome Archive (EGA) (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://ega-archive.org/submission/sequence/programmatic_submissions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>For further information, go to "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://github.com/EbiEga/ega-metadata-schema/tree/main/Star2xml#filling-out-templates</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>", where additional information regarding the filling of this template can be found.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1755,6 +1929,30 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1900,7 +2098,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -2031,12 +2229,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2210,11 +2434,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2864,124 +3098,190 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3716877C-2DD6-4C53-9859-D06BF40DA072}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="83" t="s">
-        <v>119</v>
-      </c>
-      <c r="B2" s="84"/>
+      <c r="A2" s="87" t="s">
+        <v>398</v>
+      </c>
+      <c r="B2" s="86"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>121</v>
+      <c r="A3" s="83" t="s">
+        <v>388</v>
+      </c>
+      <c r="B3" s="82" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="32">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>122</v>
+      <c r="A4" s="83" t="s">
+        <v>389</v>
+      </c>
+      <c r="B4" s="82" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="33">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>123</v>
+      <c r="A5" s="84" t="s">
+        <v>391</v>
+      </c>
+      <c r="B5" s="82" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="33">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>124</v>
+      <c r="A6" s="84" t="s">
+        <v>392</v>
+      </c>
+      <c r="B6" s="82" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="B7" t="s">
-        <v>126</v>
+      <c r="A7" s="84" t="s">
+        <v>395</v>
+      </c>
+      <c r="B7" s="82" t="s">
+        <v>394</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="83" t="s">
-        <v>127</v>
-      </c>
-      <c r="B9" s="84"/>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="84" t="s">
+        <v>397</v>
+      </c>
+      <c r="B8" s="82" t="s">
+        <v>402</v>
+      </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>121</v>
-      </c>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="88" t="s">
+        <v>404</v>
+      </c>
+      <c r="B9" s="88"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>130</v>
-      </c>
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="85" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" s="86"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>132</v>
+      <c r="A12" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>149</v>
+      <c r="A13" s="32">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
-        <v>148</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>150</v>
+      <c r="A14" s="33">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>134</v>
+      <c r="A15" s="33">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="85" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" s="86"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>386</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A18:B18"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A9:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2989,7 +3289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2EA4E3C-B110-4DC1-9919-979853C674EC}">
   <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3011,7 +3311,7 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -3020,22 +3320,22 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="G1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="H1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="I1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="J1" s="35" t="s">
         <v>0</v>
@@ -3065,33 +3365,33 @@
         <v>2</v>
       </c>
       <c r="S1" s="36" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="T1" s="36" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="U1" s="36" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="V1" s="36" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="W1" s="36" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="X1" s="36" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="Y1" s="36" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="Z1" s="36" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B2" t="s">
         <v>88</v>
@@ -3100,22 +3400,22 @@
         <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="E2" s="37" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F2" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G2" s="38" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="H2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="I2" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="J2" s="39" t="s">
         <v>5</v>
@@ -3145,28 +3445,28 @@
         <v>7</v>
       </c>
       <c r="S2" s="40" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="T2" s="40" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="U2" s="40" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="V2" s="40" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="W2" s="38" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="X2" s="38" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="Y2" s="38" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="Z2" s="38" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.25">
@@ -3177,7 +3477,7 @@
     </row>
     <row r="4" spans="1:26" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="44" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B4" s="44" t="s">
         <v>43</v>
@@ -3186,63 +3486,63 @@
         <v>35</v>
       </c>
       <c r="D4" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="G4" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="H4" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="I4" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="J4" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="K4" s="46" t="s">
         <v>174</v>
-      </c>
-      <c r="E4" s="44" t="s">
-        <v>175</v>
-      </c>
-      <c r="G4" s="37" t="s">
-        <v>176</v>
-      </c>
-      <c r="H4" s="44" t="s">
-        <v>177</v>
-      </c>
-      <c r="I4" s="44" t="s">
-        <v>178</v>
-      </c>
-      <c r="J4" s="45" t="s">
-        <v>179</v>
-      </c>
-      <c r="K4" s="46" t="s">
-        <v>180</v>
       </c>
       <c r="L4" s="46"/>
       <c r="M4" s="44" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="N4" s="44" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="P4" s="46" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="Q4" s="46" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="R4" s="46"/>
       <c r="S4" s="47" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="T4" s="47">
         <v>406</v>
       </c>
       <c r="U4" s="47" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="V4" s="48" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="W4" s="44" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="X4" s="44">
         <v>110649</v>
       </c>
       <c r="Y4" s="44" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="Z4" s="49" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
@@ -3325,7 +3625,7 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -3334,16 +3634,16 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="E1" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="F1" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="G1" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="H1" t="s">
         <v>121</v>
@@ -3405,7 +3705,7 @@
     </row>
     <row r="2" spans="1:26" s="44" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="44" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="B2" s="44" t="s">
         <v>88</v>
@@ -3414,67 +3714,67 @@
         <v>89</v>
       </c>
       <c r="D2" s="44" t="s">
+        <v>319</v>
+      </c>
+      <c r="E2" s="44" t="s">
+        <v>320</v>
+      </c>
+      <c r="F2" s="44" t="s">
+        <v>321</v>
+      </c>
+      <c r="G2" s="44" t="s">
+        <v>322</v>
+      </c>
+      <c r="H2" s="44" t="s">
+        <v>323</v>
+      </c>
+      <c r="I2" s="46" t="s">
+        <v>324</v>
+      </c>
+      <c r="J2" s="46" t="s">
         <v>325</v>
-      </c>
-      <c r="E2" s="44" t="s">
-        <v>326</v>
-      </c>
-      <c r="F2" s="44" t="s">
-        <v>327</v>
-      </c>
-      <c r="G2" s="44" t="s">
-        <v>328</v>
-      </c>
-      <c r="H2" s="44" t="s">
-        <v>329</v>
-      </c>
-      <c r="I2" s="46" t="s">
-        <v>330</v>
-      </c>
-      <c r="J2" s="46" t="s">
-        <v>331</v>
       </c>
       <c r="K2" s="46"/>
       <c r="L2" s="46" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="M2" s="75" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="N2" s="46"/>
       <c r="O2" s="46" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="P2" s="46" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="Q2" s="46"/>
       <c r="R2" s="45" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="S2" s="46" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="T2" s="46" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="U2" s="44" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="V2" s="44" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="W2" s="44" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="X2" s="46" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="Y2" s="46" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="Z2" s="46" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="3" spans="1:26" s="20" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3486,7 +3786,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="B4" t="s">
         <v>43</v>
@@ -3495,61 +3795,61 @@
         <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="E4">
         <v>9606</v>
       </c>
       <c r="F4" t="s">
+        <v>335</v>
+      </c>
+      <c r="G4" t="s">
+        <v>336</v>
+      </c>
+      <c r="H4" t="s">
+        <v>337</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="R4" s="39" t="s">
+        <v>340</v>
+      </c>
+      <c r="S4" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="G4" t="s">
+      <c r="T4" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="H4" t="s">
+      <c r="U4" t="s">
         <v>343</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="M4" s="2" t="s">
+      <c r="V4" t="s">
         <v>344</v>
       </c>
-      <c r="O4" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="P4" s="2" t="s">
+      <c r="W4" t="s">
+        <v>342</v>
+      </c>
+      <c r="X4" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="R4" s="39" t="s">
+      <c r="Y4" s="2" t="s">
         <v>346</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="U4" t="s">
-        <v>349</v>
-      </c>
-      <c r="V4" t="s">
-        <v>350</v>
-      </c>
-      <c r="W4" t="s">
-        <v>348</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -3605,7 +3905,7 @@
   <sheetData>
     <row r="1" spans="1:61" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -3614,10 +3914,10 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="F1" t="s">
         <v>8</v>
@@ -3626,70 +3926,70 @@
         <v>121</v>
       </c>
       <c r="H1" t="s">
+        <v>187</v>
+      </c>
+      <c r="I1" t="s">
+        <v>188</v>
+      </c>
+      <c r="J1" s="51" t="s">
+        <v>189</v>
+      </c>
+      <c r="K1" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="L1" s="51" t="s">
+        <v>191</v>
+      </c>
+      <c r="M1" s="51" t="s">
+        <v>192</v>
+      </c>
+      <c r="N1" s="51" t="s">
         <v>193</v>
       </c>
-      <c r="I1" t="s">
+      <c r="O1" s="51" t="s">
         <v>194</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="P1" s="51" t="s">
         <v>195</v>
       </c>
-      <c r="K1" s="51" t="s">
+      <c r="Q1" s="51" t="s">
         <v>196</v>
       </c>
-      <c r="L1" s="51" t="s">
+      <c r="R1" s="51" t="s">
         <v>197</v>
       </c>
-      <c r="M1" s="51" t="s">
+      <c r="S1" s="51" t="s">
         <v>198</v>
       </c>
-      <c r="N1" s="51" t="s">
+      <c r="T1" s="51" t="s">
         <v>199</v>
       </c>
-      <c r="O1" s="51" t="s">
+      <c r="U1" s="51" t="s">
         <v>200</v>
       </c>
-      <c r="P1" s="51" t="s">
+      <c r="V1" s="51" t="s">
         <v>201</v>
       </c>
-      <c r="Q1" s="51" t="s">
+      <c r="W1" s="51" t="s">
         <v>202</v>
       </c>
-      <c r="R1" s="51" t="s">
+      <c r="X1" s="51" t="s">
         <v>203</v>
       </c>
-      <c r="S1" s="51" t="s">
+      <c r="Y1" s="51" t="s">
         <v>204</v>
       </c>
-      <c r="T1" s="51" t="s">
+      <c r="Z1" s="51" t="s">
         <v>205</v>
       </c>
-      <c r="U1" s="51" t="s">
+      <c r="AA1" s="51" t="s">
         <v>206</v>
       </c>
-      <c r="V1" s="51" t="s">
+      <c r="AB1" s="51" t="s">
         <v>207</v>
       </c>
-      <c r="W1" s="51" t="s">
+      <c r="AC1" s="51" t="s">
         <v>208</v>
-      </c>
-      <c r="X1" s="51" t="s">
-        <v>209</v>
-      </c>
-      <c r="Y1" s="51" t="s">
-        <v>210</v>
-      </c>
-      <c r="Z1" s="51" t="s">
-        <v>211</v>
-      </c>
-      <c r="AA1" s="51" t="s">
-        <v>212</v>
-      </c>
-      <c r="AB1" s="51" t="s">
-        <v>213</v>
-      </c>
-      <c r="AC1" s="51" t="s">
-        <v>214</v>
       </c>
       <c r="AD1" s="52" t="s">
         <v>0</v>
@@ -3701,96 +4001,96 @@
         <v>2</v>
       </c>
       <c r="AG1" s="53" t="s">
+        <v>209</v>
+      </c>
+      <c r="AH1" s="53" t="s">
+        <v>210</v>
+      </c>
+      <c r="AI1" s="53" t="s">
+        <v>209</v>
+      </c>
+      <c r="AJ1" s="53" t="s">
+        <v>210</v>
+      </c>
+      <c r="AK1" s="53" t="s">
+        <v>209</v>
+      </c>
+      <c r="AL1" s="53" t="s">
+        <v>210</v>
+      </c>
+      <c r="AM1" s="54" t="s">
+        <v>211</v>
+      </c>
+      <c r="AN1" s="54" t="s">
+        <v>212</v>
+      </c>
+      <c r="AO1" s="54" t="s">
+        <v>213</v>
+      </c>
+      <c r="AP1" s="54" t="s">
+        <v>214</v>
+      </c>
+      <c r="AQ1" s="54" t="s">
         <v>215</v>
       </c>
-      <c r="AH1" s="53" t="s">
+      <c r="AR1" s="54" t="s">
         <v>216</v>
       </c>
-      <c r="AI1" s="53" t="s">
+      <c r="AS1" s="54" t="s">
+        <v>211</v>
+      </c>
+      <c r="AT1" s="54" t="s">
+        <v>212</v>
+      </c>
+      <c r="AU1" s="54" t="s">
+        <v>213</v>
+      </c>
+      <c r="AV1" s="54" t="s">
+        <v>214</v>
+      </c>
+      <c r="AW1" s="54" t="s">
         <v>215</v>
       </c>
-      <c r="AJ1" s="53" t="s">
+      <c r="AX1" s="54" t="s">
         <v>216</v>
       </c>
-      <c r="AK1" s="53" t="s">
-        <v>215</v>
-      </c>
-      <c r="AL1" s="53" t="s">
-        <v>216</v>
-      </c>
-      <c r="AM1" s="54" t="s">
+      <c r="AY1" s="55" t="s">
         <v>217</v>
       </c>
-      <c r="AN1" s="54" t="s">
+      <c r="AZ1" s="55" t="s">
         <v>218</v>
       </c>
-      <c r="AO1" s="54" t="s">
+      <c r="BA1" s="55" t="s">
+        <v>217</v>
+      </c>
+      <c r="BB1" s="55" t="s">
+        <v>218</v>
+      </c>
+      <c r="BC1" s="55" t="s">
+        <v>217</v>
+      </c>
+      <c r="BD1" s="55" t="s">
+        <v>218</v>
+      </c>
+      <c r="BE1" s="56" t="s">
         <v>219</v>
       </c>
-      <c r="AP1" s="54" t="s">
+      <c r="BF1" s="56" t="s">
         <v>220</v>
       </c>
-      <c r="AQ1" s="54" t="s">
+      <c r="BG1" s="57" t="s">
         <v>221</v>
       </c>
-      <c r="AR1" s="54" t="s">
+      <c r="BH1" s="57" t="s">
         <v>222</v>
       </c>
-      <c r="AS1" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="AT1" s="54" t="s">
-        <v>218</v>
-      </c>
-      <c r="AU1" s="54" t="s">
-        <v>219</v>
-      </c>
-      <c r="AV1" s="54" t="s">
-        <v>220</v>
-      </c>
-      <c r="AW1" s="54" t="s">
-        <v>221</v>
-      </c>
-      <c r="AX1" s="54" t="s">
-        <v>222</v>
-      </c>
-      <c r="AY1" s="55" t="s">
+      <c r="BI1" s="58" t="s">
         <v>223</v>
-      </c>
-      <c r="AZ1" s="55" t="s">
-        <v>224</v>
-      </c>
-      <c r="BA1" s="55" t="s">
-        <v>223</v>
-      </c>
-      <c r="BB1" s="55" t="s">
-        <v>224</v>
-      </c>
-      <c r="BC1" s="55" t="s">
-        <v>223</v>
-      </c>
-      <c r="BD1" s="55" t="s">
-        <v>224</v>
-      </c>
-      <c r="BE1" s="56" t="s">
-        <v>225</v>
-      </c>
-      <c r="BF1" s="56" t="s">
-        <v>226</v>
-      </c>
-      <c r="BG1" s="57" t="s">
-        <v>227</v>
-      </c>
-      <c r="BH1" s="57" t="s">
-        <v>228</v>
-      </c>
-      <c r="BI1" s="58" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:61" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B2" t="s">
         <v>88</v>
@@ -3799,82 +4099,82 @@
         <v>89</v>
       </c>
       <c r="D2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>226</v>
+      </c>
+      <c r="F2" t="s">
+        <v>227</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>228</v>
+      </c>
+      <c r="H2" t="s">
+        <v>229</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>230</v>
+      </c>
+      <c r="J2" s="37" t="s">
         <v>231</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="K2" s="37" t="s">
         <v>232</v>
       </c>
-      <c r="F2" t="s">
+      <c r="L2" s="38" t="s">
         <v>233</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="M2" t="s">
         <v>234</v>
       </c>
-      <c r="H2" t="s">
+      <c r="N2" t="s">
         <v>235</v>
       </c>
-      <c r="I2" s="37" t="s">
+      <c r="O2" t="s">
         <v>236</v>
       </c>
-      <c r="J2" s="37" t="s">
+      <c r="P2" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="K2" s="37" t="s">
+      <c r="Q2" t="s">
         <v>238</v>
       </c>
-      <c r="L2" s="38" t="s">
+      <c r="R2" t="s">
         <v>239</v>
       </c>
-      <c r="M2" t="s">
+      <c r="S2" t="s">
         <v>240</v>
       </c>
-      <c r="N2" t="s">
+      <c r="T2" s="38" t="s">
         <v>241</v>
       </c>
-      <c r="O2" t="s">
+      <c r="U2" t="s">
         <v>242</v>
       </c>
-      <c r="P2" s="38" t="s">
+      <c r="V2" t="s">
         <v>243</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="W2" t="s">
         <v>244</v>
       </c>
-      <c r="R2" t="s">
+      <c r="X2" t="s">
         <v>245</v>
       </c>
-      <c r="S2" t="s">
+      <c r="Y2" t="s">
         <v>246</v>
       </c>
-      <c r="T2" s="38" t="s">
+      <c r="Z2" t="s">
         <v>247</v>
       </c>
-      <c r="U2" t="s">
+      <c r="AA2" s="38" t="s">
         <v>248</v>
       </c>
-      <c r="V2" t="s">
+      <c r="AB2" t="s">
         <v>249</v>
       </c>
-      <c r="W2" t="s">
+      <c r="AC2" t="s">
         <v>250</v>
-      </c>
-      <c r="X2" t="s">
-        <v>251</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>252</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>253</v>
-      </c>
-      <c r="AA2" s="38" t="s">
-        <v>254</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>255</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>256</v>
       </c>
       <c r="AD2" s="59" t="s">
         <v>5</v>
@@ -3886,91 +4186,91 @@
         <v>7</v>
       </c>
       <c r="AG2" s="60" t="s">
+        <v>251</v>
+      </c>
+      <c r="AH2" s="60" t="s">
+        <v>252</v>
+      </c>
+      <c r="AI2" s="38" t="s">
+        <v>251</v>
+      </c>
+      <c r="AJ2" s="38" t="s">
+        <v>252</v>
+      </c>
+      <c r="AK2" s="60" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL2" s="60" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM2" s="61" t="s">
+        <v>253</v>
+      </c>
+      <c r="AN2" s="62" t="s">
+        <v>254</v>
+      </c>
+      <c r="AO2" s="61" t="s">
+        <v>255</v>
+      </c>
+      <c r="AP2" s="61" t="s">
+        <v>256</v>
+      </c>
+      <c r="AQ2" s="61" t="s">
         <v>257</v>
       </c>
-      <c r="AH2" s="60" t="s">
+      <c r="AR2" s="61" t="s">
         <v>258</v>
       </c>
-      <c r="AI2" s="38" t="s">
+      <c r="AS2" t="s">
+        <v>253</v>
+      </c>
+      <c r="AT2" s="38" t="s">
+        <v>259</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>255</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>256</v>
+      </c>
+      <c r="AW2" t="s">
         <v>257</v>
       </c>
-      <c r="AJ2" s="38" t="s">
+      <c r="AX2" t="s">
         <v>258</v>
       </c>
-      <c r="AK2" s="60" t="s">
-        <v>257</v>
-      </c>
-      <c r="AL2" s="60" t="s">
-        <v>258</v>
-      </c>
-      <c r="AM2" s="61" t="s">
-        <v>259</v>
-      </c>
-      <c r="AN2" s="62" t="s">
+      <c r="AY2" s="63" t="s">
         <v>260</v>
       </c>
-      <c r="AO2" s="61" t="s">
+      <c r="AZ2" s="63" t="s">
         <v>261</v>
       </c>
-      <c r="AP2" s="61" t="s">
+      <c r="BA2" t="s">
+        <v>260</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>261</v>
+      </c>
+      <c r="BC2" s="63" t="s">
+        <v>260</v>
+      </c>
+      <c r="BD2" s="63" t="s">
+        <v>261</v>
+      </c>
+      <c r="BE2" t="s">
         <v>262</v>
       </c>
-      <c r="AQ2" s="61" t="s">
+      <c r="BF2" t="s">
         <v>263</v>
       </c>
-      <c r="AR2" s="61" t="s">
+      <c r="BG2" t="s">
         <v>264</v>
       </c>
-      <c r="AS2" t="s">
-        <v>259</v>
-      </c>
-      <c r="AT2" s="38" t="s">
+      <c r="BH2" t="s">
         <v>265</v>
       </c>
-      <c r="AU2" t="s">
-        <v>261</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>262</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>263</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>264</v>
-      </c>
-      <c r="AY2" s="63" t="s">
+      <c r="BI2" t="s">
         <v>266</v>
-      </c>
-      <c r="AZ2" s="63" t="s">
-        <v>267</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>266</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>267</v>
-      </c>
-      <c r="BC2" s="63" t="s">
-        <v>266</v>
-      </c>
-      <c r="BD2" s="63" t="s">
-        <v>267</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>268</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>269</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>270</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>271</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:61" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3981,7 +4281,7 @@
     </row>
     <row r="4" spans="1:61" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="B4" t="s">
         <v>43</v>
@@ -3990,160 +4290,160 @@
         <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E4" t="s">
         <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="G4" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="H4" t="s">
         <v>42</v>
       </c>
       <c r="I4" t="s">
+        <v>271</v>
+      </c>
+      <c r="J4" t="s">
+        <v>272</v>
+      </c>
+      <c r="K4" t="s">
+        <v>273</v>
+      </c>
+      <c r="L4" t="s">
+        <v>274</v>
+      </c>
+      <c r="M4" t="s">
+        <v>275</v>
+      </c>
+      <c r="N4" t="s">
+        <v>276</v>
+      </c>
+      <c r="O4" t="s">
         <v>277</v>
       </c>
-      <c r="J4" t="s">
+      <c r="P4" t="s">
         <v>278</v>
-      </c>
-      <c r="K4" t="s">
-        <v>279</v>
-      </c>
-      <c r="L4" t="s">
-        <v>280</v>
-      </c>
-      <c r="M4" t="s">
-        <v>281</v>
-      </c>
-      <c r="N4" t="s">
-        <v>282</v>
-      </c>
-      <c r="O4" t="s">
-        <v>283</v>
-      </c>
-      <c r="P4" t="s">
-        <v>284</v>
       </c>
       <c r="Q4">
         <v>80</v>
       </c>
       <c r="R4" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="S4">
         <v>10</v>
       </c>
       <c r="T4" t="s">
+        <v>280</v>
+      </c>
+      <c r="U4" t="s">
+        <v>281</v>
+      </c>
+      <c r="V4" s="64" t="s">
+        <v>183</v>
+      </c>
+      <c r="W4" s="65" t="s">
+        <v>282</v>
+      </c>
+      <c r="X4" t="s">
+        <v>283</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>284</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>285</v>
+      </c>
+      <c r="AA4" t="s">
         <v>286</v>
       </c>
-      <c r="U4" t="s">
+      <c r="AB4" t="s">
         <v>287</v>
       </c>
-      <c r="V4" s="64" t="s">
-        <v>189</v>
-      </c>
-      <c r="W4" s="65" t="s">
+      <c r="AC4" t="s">
         <v>288</v>
       </c>
-      <c r="X4" t="s">
+      <c r="AD4" s="59" t="s">
         <v>289</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="AE4" s="66" t="s">
         <v>290</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AG4" s="67" t="s">
         <v>291</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AH4" s="67" t="s">
         <v>292</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AI4" t="s">
         <v>293</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AJ4" t="s">
         <v>294</v>
       </c>
-      <c r="AD4" s="59" t="s">
+      <c r="AK4" s="67" t="s">
         <v>295</v>
       </c>
-      <c r="AE4" s="66" t="s">
+      <c r="AL4" s="67" t="s">
         <v>296</v>
       </c>
-      <c r="AG4" s="67" t="s">
+      <c r="AM4" s="61" t="s">
         <v>297</v>
       </c>
-      <c r="AH4" s="67" t="s">
+      <c r="AN4" s="61" t="s">
         <v>298</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AO4" s="61" t="s">
+        <v>255</v>
+      </c>
+      <c r="AP4" s="61" t="s">
         <v>299</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AQ4" s="61" t="s">
         <v>300</v>
       </c>
-      <c r="AK4" s="67" t="s">
+      <c r="AS4" t="s">
         <v>301</v>
       </c>
-      <c r="AL4" s="67" t="s">
+      <c r="AT4" t="s">
         <v>302</v>
       </c>
-      <c r="AM4" s="61" t="s">
+      <c r="AU4" t="s">
+        <v>255</v>
+      </c>
+      <c r="AV4" t="s">
         <v>303</v>
       </c>
-      <c r="AN4" s="61" t="s">
+      <c r="AW4" t="s">
         <v>304</v>
       </c>
-      <c r="AO4" s="61" t="s">
-        <v>261</v>
-      </c>
-      <c r="AP4" s="61" t="s">
+      <c r="AY4" s="63" t="s">
         <v>305</v>
       </c>
-      <c r="AQ4" s="61" t="s">
+      <c r="BA4" t="s">
         <v>306</v>
       </c>
-      <c r="AS4" t="s">
+      <c r="BB4" t="s">
         <v>307</v>
       </c>
-      <c r="AT4" t="s">
+      <c r="BC4" s="63" t="s">
         <v>308</v>
       </c>
-      <c r="AU4" t="s">
-        <v>261</v>
-      </c>
-      <c r="AV4" t="s">
+      <c r="BE4" t="s">
         <v>309</v>
       </c>
-      <c r="AW4" t="s">
+      <c r="BG4" t="s">
         <v>310</v>
       </c>
-      <c r="AY4" s="63" t="s">
+      <c r="BH4" t="s">
         <v>311</v>
       </c>
-      <c r="BA4" t="s">
+      <c r="BI4" t="s">
         <v>312</v>
-      </c>
-      <c r="BB4" t="s">
-        <v>313</v>
-      </c>
-      <c r="BC4" s="63" t="s">
-        <v>314</v>
-      </c>
-      <c r="BE4" t="s">
-        <v>315</v>
-      </c>
-      <c r="BG4" t="s">
-        <v>316</v>
-      </c>
-      <c r="BH4" t="s">
-        <v>317</v>
-      </c>
-      <c r="BI4" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="17" spans="6:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4293,13 +4593,13 @@
         <v>29</v>
       </c>
       <c r="M1" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="P1" s="9" t="s">
         <v>30</v>
@@ -4311,7 +4611,7 @@
         <v>32</v>
       </c>
       <c r="S1" s="9" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>9</v>
@@ -4469,13 +4769,13 @@
         <v>101</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="O2" s="29" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>102</v>
@@ -4487,7 +4787,7 @@
         <v>33</v>
       </c>
       <c r="S2" s="18" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="T2" s="7" t="s">
         <v>103</v>
@@ -4562,7 +4862,7 @@
         <v>70</v>
       </c>
       <c r="AR2" s="16" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="AS2" s="16" t="s">
         <v>71</v>
@@ -4654,7 +4954,7 @@
         <v>41</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="N4" s="8">
         <v>390</v>
@@ -4672,7 +4972,7 @@
         <v>51</v>
       </c>
       <c r="S4" s="18" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="U4" s="1" t="s">
         <v>44</v>
@@ -4681,7 +4981,7 @@
         <v>1</v>
       </c>
       <c r="AR4" s="16" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="AS4" s="16" t="s">
         <v>75</v>
@@ -4806,7 +5106,7 @@
   <sheetData>
     <row r="1" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -4815,22 +5115,22 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="E1" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="F1" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="82" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="H1" s="51" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="I1" s="51" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="J1" s="35" t="s">
         <v>0</v>
@@ -4851,75 +5151,75 @@
         <v>2</v>
       </c>
       <c r="P1" s="53" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q1" s="53" t="s">
+        <v>210</v>
+      </c>
+      <c r="R1" s="53" t="s">
+        <v>209</v>
+      </c>
+      <c r="S1" s="53" t="s">
+        <v>210</v>
+      </c>
+      <c r="T1" s="53" t="s">
+        <v>209</v>
+      </c>
+      <c r="U1" s="53" t="s">
+        <v>210</v>
+      </c>
+      <c r="V1" s="54" t="s">
+        <v>211</v>
+      </c>
+      <c r="W1" s="54" t="s">
+        <v>212</v>
+      </c>
+      <c r="X1" s="54" t="s">
+        <v>213</v>
+      </c>
+      <c r="Y1" s="54" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z1" s="54" t="s">
         <v>215</v>
       </c>
-      <c r="Q1" s="53" t="s">
-        <v>216</v>
-      </c>
-      <c r="R1" s="53" t="s">
+      <c r="AA1" s="54" t="s">
+        <v>351</v>
+      </c>
+      <c r="AB1" s="54" t="s">
+        <v>352</v>
+      </c>
+      <c r="AC1" s="54" t="s">
+        <v>353</v>
+      </c>
+      <c r="AD1" s="54" t="s">
+        <v>211</v>
+      </c>
+      <c r="AE1" s="54" t="s">
+        <v>212</v>
+      </c>
+      <c r="AF1" s="54" t="s">
+        <v>213</v>
+      </c>
+      <c r="AG1" s="54" t="s">
+        <v>214</v>
+      </c>
+      <c r="AH1" s="54" t="s">
         <v>215</v>
       </c>
-      <c r="S1" s="53" t="s">
-        <v>216</v>
-      </c>
-      <c r="T1" s="53" t="s">
-        <v>215</v>
-      </c>
-      <c r="U1" s="53" t="s">
-        <v>216</v>
-      </c>
-      <c r="V1" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="W1" s="54" t="s">
-        <v>218</v>
-      </c>
-      <c r="X1" s="54" t="s">
-        <v>219</v>
-      </c>
-      <c r="Y1" s="54" t="s">
-        <v>220</v>
-      </c>
-      <c r="Z1" s="54" t="s">
-        <v>221</v>
-      </c>
-      <c r="AA1" s="54" t="s">
-        <v>357</v>
-      </c>
-      <c r="AB1" s="54" t="s">
-        <v>358</v>
-      </c>
-      <c r="AC1" s="54" t="s">
-        <v>359</v>
-      </c>
-      <c r="AD1" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="AE1" s="54" t="s">
-        <v>218</v>
-      </c>
-      <c r="AF1" s="54" t="s">
-        <v>219</v>
-      </c>
-      <c r="AG1" s="54" t="s">
-        <v>220</v>
-      </c>
-      <c r="AH1" s="54" t="s">
-        <v>221</v>
-      </c>
       <c r="AI1" s="54" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="AJ1" s="54" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="AK1" s="54" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
     </row>
     <row r="2" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="B2" t="s">
         <v>88</v>
@@ -4928,22 +5228,22 @@
         <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E2" s="37" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="F2" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="G2" s="38" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="H2" s="38" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="I2" s="38" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="J2" s="39" t="s">
         <v>5</v>
@@ -4964,70 +5264,70 @@
         <v>7</v>
       </c>
       <c r="P2" s="60" t="s">
+        <v>361</v>
+      </c>
+      <c r="Q2" s="60" t="s">
+        <v>362</v>
+      </c>
+      <c r="R2" s="38" t="s">
+        <v>361</v>
+      </c>
+      <c r="S2" s="38" t="s">
+        <v>362</v>
+      </c>
+      <c r="T2" s="60" t="s">
+        <v>361</v>
+      </c>
+      <c r="U2" s="60" t="s">
+        <v>362</v>
+      </c>
+      <c r="V2" s="77" t="s">
+        <v>363</v>
+      </c>
+      <c r="W2" s="77" t="s">
+        <v>364</v>
+      </c>
+      <c r="X2" s="78" t="s">
+        <v>255</v>
+      </c>
+      <c r="Y2" s="78" t="s">
+        <v>256</v>
+      </c>
+      <c r="Z2" s="78" t="s">
+        <v>257</v>
+      </c>
+      <c r="AA2" s="78" t="s">
+        <v>365</v>
+      </c>
+      <c r="AB2" s="78" t="s">
+        <v>366</v>
+      </c>
+      <c r="AC2" s="78" t="s">
         <v>367</v>
       </c>
-      <c r="Q2" s="60" t="s">
+      <c r="AD2" s="38" t="s">
+        <v>363</v>
+      </c>
+      <c r="AE2" s="38" t="s">
+        <v>364</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>255</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>256</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>257</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>365</v>
+      </c>
+      <c r="AJ2" t="s">
         <v>368</v>
       </c>
-      <c r="R2" s="38" t="s">
+      <c r="AK2" t="s">
         <v>367</v>
-      </c>
-      <c r="S2" s="38" t="s">
-        <v>368</v>
-      </c>
-      <c r="T2" s="60" t="s">
-        <v>367</v>
-      </c>
-      <c r="U2" s="60" t="s">
-        <v>368</v>
-      </c>
-      <c r="V2" s="77" t="s">
-        <v>369</v>
-      </c>
-      <c r="W2" s="77" t="s">
-        <v>370</v>
-      </c>
-      <c r="X2" s="78" t="s">
-        <v>261</v>
-      </c>
-      <c r="Y2" s="78" t="s">
-        <v>262</v>
-      </c>
-      <c r="Z2" s="78" t="s">
-        <v>263</v>
-      </c>
-      <c r="AA2" s="78" t="s">
-        <v>371</v>
-      </c>
-      <c r="AB2" s="78" t="s">
-        <v>372</v>
-      </c>
-      <c r="AC2" s="78" t="s">
-        <v>373</v>
-      </c>
-      <c r="AD2" s="38" t="s">
-        <v>369</v>
-      </c>
-      <c r="AE2" s="38" t="s">
-        <v>370</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>261</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>262</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>263</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>371</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>374</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="3" spans="1:37" s="80" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5038,7 +5338,7 @@
     </row>
     <row r="4" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="B4" t="s">
         <v>43</v>
@@ -5047,100 +5347,100 @@
         <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="E4" t="s">
         <v>43</v>
       </c>
       <c r="F4" t="s">
+        <v>371</v>
+      </c>
+      <c r="G4" t="s">
+        <v>372</v>
+      </c>
+      <c r="H4" t="s">
+        <v>272</v>
+      </c>
+      <c r="I4" t="s">
+        <v>273</v>
+      </c>
+      <c r="J4" s="39" t="s">
+        <v>373</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="M4" t="s">
+        <v>375</v>
+      </c>
+      <c r="N4" t="s">
+        <v>376</v>
+      </c>
+      <c r="P4" s="67" t="s">
+        <v>291</v>
+      </c>
+      <c r="Q4" s="67" t="s">
+        <v>292</v>
+      </c>
+      <c r="R4" t="s">
+        <v>293</v>
+      </c>
+      <c r="S4" t="s">
+        <v>294</v>
+      </c>
+      <c r="T4" s="67" t="s">
+        <v>295</v>
+      </c>
+      <c r="U4" s="67" t="s">
+        <v>296</v>
+      </c>
+      <c r="V4" s="78" t="s">
         <v>377</v>
       </c>
-      <c r="G4" t="s">
+      <c r="W4" s="78" t="s">
+        <v>298</v>
+      </c>
+      <c r="X4" s="78" t="s">
+        <v>255</v>
+      </c>
+      <c r="Y4" s="78" t="s">
+        <v>303</v>
+      </c>
+      <c r="Z4" s="78" t="s">
+        <v>304</v>
+      </c>
+      <c r="AA4" s="78" t="s">
         <v>378</v>
       </c>
-      <c r="H4" t="s">
-        <v>278</v>
-      </c>
-      <c r="I4" t="s">
-        <v>279</v>
-      </c>
-      <c r="J4" s="39" t="s">
+      <c r="AB4" s="78" t="s">
         <v>379</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="AC4" s="78" t="s">
         <v>380</v>
       </c>
-      <c r="M4" t="s">
+      <c r="AD4" t="s">
         <v>381</v>
       </c>
-      <c r="N4" t="s">
+      <c r="AE4" t="s">
         <v>382</v>
       </c>
-      <c r="P4" s="67" t="s">
-        <v>297</v>
-      </c>
-      <c r="Q4" s="67" t="s">
-        <v>298</v>
-      </c>
-      <c r="R4" t="s">
-        <v>299</v>
-      </c>
-      <c r="S4" t="s">
-        <v>300</v>
-      </c>
-      <c r="T4" s="67" t="s">
-        <v>301</v>
-      </c>
-      <c r="U4" s="67" t="s">
-        <v>302</v>
-      </c>
-      <c r="V4" s="78" t="s">
+      <c r="AF4" t="s">
+        <v>255</v>
+      </c>
+      <c r="AG4" t="s">
         <v>383</v>
       </c>
-      <c r="W4" s="78" t="s">
-        <v>304</v>
-      </c>
-      <c r="X4" s="78" t="s">
-        <v>261</v>
-      </c>
-      <c r="Y4" s="78" t="s">
-        <v>309</v>
-      </c>
-      <c r="Z4" s="78" t="s">
-        <v>310</v>
-      </c>
-      <c r="AA4" s="78" t="s">
+      <c r="AH4" t="s">
         <v>384</v>
       </c>
-      <c r="AB4" s="78" t="s">
-        <v>385</v>
-      </c>
-      <c r="AC4" s="78" t="s">
-        <v>386</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>387</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>388</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>261</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>389</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>390</v>
-      </c>
       <c r="AI4" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="AJ4" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="AK4" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EE-1836 - Updated Whole submission template Minor changes in the whole submission template file.
</commit_message>
<xml_diff>
--- a/templates/sequence-based-metadata/whole_submission_template.xlsx
+++ b/templates/sequence-based-metadata/whole_submission_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcasado\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcasado\Documents\GitHub\ega-metadata-schema\templates\sequence-based-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B603BEAF-F063-4D25-BE2A-6EB53080DA39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7020ACB7-8ACA-481E-80B8-CE3E69C137F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -199,39 +199,6 @@
     <t>SPOT_LENGTH</t>
   </si>
   <si>
-    <t>ReadSpec.READ_INDEX</t>
-  </si>
-  <si>
-    <t>ReadSpec.BASE_COORD</t>
-  </si>
-  <si>
-    <t>ReadSpec.READ_CLASS</t>
-  </si>
-  <si>
-    <t>ReadSpec.READ_TYPE</t>
-  </si>
-  <si>
-    <t>ReadSpec.Expected_Default_Length</t>
-  </si>
-  <si>
-    <t>ReadSpec.Basecall_min_match</t>
-  </si>
-  <si>
-    <t>ReadSpec.Basecall_max_mismatch</t>
-  </si>
-  <si>
-    <t>ReadSpec.Basecall_match_edge</t>
-  </si>
-  <si>
-    <t>ReadSpec.Basecall</t>
-  </si>
-  <si>
-    <t>ReadSpec.READ_LABEL</t>
-  </si>
-  <si>
-    <t>ReadSpec.Preceding_read_index</t>
-  </si>
-  <si>
     <t>Pipeline.StepIndex</t>
   </si>
   <si>
@@ -278,9 +245,6 @@
   </si>
   <si>
     <t>Image Analysis 1.3.4 - set birghtness to 30% through command X</t>
-  </si>
-  <si>
-    <t>TODO: the class of the read, either 'Application Read' or 'Technical Read'.</t>
   </si>
   <si>
     <t>TODO: Number of base/color calls, cycles, or flows per spot (e.g. 102) (raw sequence length or flow length including all application and technical tags and mate pairs, but not including gap lengths). This value will be platform dependent, library dependent, and possibly run dependent. Variable length platforms will still have a constant flow/cycle length.</t>
@@ -964,175 +928,6 @@
 	Target sequencing</t>
   </si>
   <si>
-    <t>#! This will be changed once EE-1836 is done -- TODO: Programs used (comma separated, and with their version if applicable). Use this column exclusively if the Analysis is of type Sequence Variation.</t>
-  </si>
-  <si>
-    <t>#! This will be changed once EE-1836 is done -- TODO: Use this column exclusively if the Analysis is of type Sequence Variation.</t>
-  </si>
-  <si>
-    <t>#! This will be changed once EE-1836 is done -- TODO: Name of the Sequence Assembly. Only use this column if the Analysis is of type Sequence Assembly.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">#! This will be changed once EE-1836 is done -- TODO: Type of the Sequence assembly. Only use this column if the Analysis is of type Sequence Assembly. Must be value from Controlled vocabulary (description in parenthesis):
-	clone or isolate                (An assembly of reads from an isolated cultured organism, tissues, cells or a cell line)
-	</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>primary metagenome</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                (An original metagenome assembly prior to binning from a sampled biome or collection of sampled biomes without attempt to separate taxa)
-	</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>binned metagenome</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                (A set of contigs drawn from primary or unbinned metagenomes grouped into a single-taxon set)
-	</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Metagenome-Assembled Genome (MAG)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                (A single-taxon assembly based on a binned metagenome asserted to be a close representation to an actual individual genome (that could match an already existing isolate or represent a novel isolate))
-	</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Environmental Single-Cell Amplified Genome (SAG)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                (A genome assembly from amplified environmental sampled single-cell DNA)
-	</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>COVID-19 outbreak</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                (A genome assembly specific to COVID-19 outbreak)</t>
-    </r>
-  </si>
-  <si>
-    <t>#! This will be changed once EE-1836 is done -- TODO: Coverage of the Sequence Assembly. Only use this column if the Analysis is of type Sequence Assembly.</t>
-  </si>
-  <si>
-    <t>#! This will be changed once EE-1836 is done -- TODO: Platform used for the Sequence Assembly. Only use this column if the Analysis is of type Sequence Assembly.</t>
-  </si>
-  <si>
-    <t>#! This will be changed once EE-1836 is done -- TODO: Minimum Gap length used of the Sequence Assembly. Only use this column if the Analysis is of type Sequence Assembly.</t>
-  </si>
-  <si>
-    <t>#! This will be changed once EE-1836 is done -- TODO: Molecule type used in the Sequence Assembly. Only use this column if the Analysis is of type Sequence Assembly. Must be value from Controlled vocabulary:
-	genomic DNA
-	genomic RNA
-	viral cRNA</t>
-  </si>
-  <si>
-    <t>#! This will be changed once EE-1836 is done -- TODO: Program used for the Sequence Assembly. Only use this column if the Analysis is of type Sequence Assembly.</t>
-  </si>
-  <si>
-    <t>#! This will be changed once EE-1836 is done -- TODO: Specifies if the Sequence assembly is partial or not (use 'True' or 'False'). Only use this column if the Analysis is of type Sequence Assembly.</t>
-  </si>
-  <si>
-    <t>#! This will be changed once EE-1836 is done -- TODO: Program used for the Genome Mapping. Use this column exclusively if the Analysis is of type Genome Map.</t>
-  </si>
-  <si>
-    <t>#! This will be changed once EE-1836 is done -- TODO: Platform used for the Genome Mapping. Use this column exclusively if the Analysis is of type Genome Map.</t>
-  </si>
-  <si>
-    <t>#! This will be changed once EE-1836 is done -- TODO: Description of the Genome Map. Use this column exclusively if the Analysis is of type Genome Map.</t>
-  </si>
-  <si>
-    <t>#! This will be changed once EE-1836 is done -- TODO: Name of the transcriptome assembly. Use this column exclusively if the Analysis is of type Transcriptome Assembly.</t>
-  </si>
-  <si>
-    <t>#! This will be changed once EE-1836 is done -- TODO: Type of the transcriptome assembly. Use this column exclusively if the Analysis is of type Transcriptome Assembly. Must be value from Controlled vocabulary: 
-	isolate
-	metatranscriptome</t>
-  </si>
-  <si>
-    <t>#! This will be changed once EE-1836 is done -- TODO: Platform used for the transcriptome assembly. Use this column exclusively if the Analysis is of type Transcriptome Assembly.</t>
-  </si>
-  <si>
-    <t>#! This will be changed once EE-1836 is done -- TODO: Program used for the transcriptome assembly. Use this column exclusively if the Analysis is of type Transcriptome Assembly.</t>
-  </si>
-  <si>
     <t xml:space="preserve">TODO: Accession of the sequence for the reference alignment in format 'Accession.version', with version being mandatory (e.g. CM000663.1). Use this column exclusively if the Analysis is of type REFERENCE_ALIGNMENT, SEQUENCE_VARIATION, SEQUENCE_ANNOTATION or PROCESSED_READS
 In case you want to provide several sequence details, repeat the block 'SEQUENCE.Accession' - 'SEQUENCE.Label' as many times as needed. </t>
   </si>
@@ -1621,60 +1416,108 @@
     <t>9ddd9749fdc4118a2c614140cea6c7c3</t>
   </si>
   <si>
-    <t>Optional ( yet highly recommended) attributes</t>
-  </si>
-  <si>
-    <t>Repeated blocks (each with their own colour): you can add or remove as many "whole" blocks as you want to fulfil your needs, but remember to always work with complete repetitions (e.g. adding three new columns TAG-VALUE-UNITS for a new attribute, but not adding only one or two of them TAG-VALUE)</t>
-  </si>
-  <si>
-    <t>Real data "ceiling" (put your real data beneath this row)</t>
+    <t>TODO: Programs used (comma separated, and with their version if applicable). Use this column exclusively if the Analysis is of type Sequence Variation.</t>
+  </si>
+  <si>
+    <t>TODO: Use this column exclusively if the Analysis is of type Sequence Variation.</t>
+  </si>
+  <si>
+    <t>TODO: Name of the Sequence Assembly. Only use this column if the Analysis is of type Sequence Assembly.</t>
+  </si>
+  <si>
+    <t>TODO: Type of the Sequence assembly. Only use this column if the Analysis is of type Sequence Assembly. Must be value from Controlled vocabulary (description in parenthesis):
+	clone or isolate                (An assembly of reads from an isolated cultured organism, tissues, cells or a cell line)
+	primary metagenome                (An original metagenome assembly prior to binning from a sampled biome or collection of sampled biomes without attempt to separate taxa)
+	binned metagenome                (A set of contigs drawn from primary or unbinned metagenomes grouped into a single-taxon set)
+	Metagenome-Assembled Genome (MAG)                (A single-taxon assembly based on a binned metagenome asserted to be a close representation to an actual individual genome (that could match an already existing isolate or represent a novel isolate))
+	Environmental Single-Cell Amplified Genome (SAG)                (A genome assembly from amplified environmental sampled single-cell DNA)
+	COVID-19 outbreak                (A genome assembly specific to COVID-19 outbreak)</t>
+  </si>
+  <si>
+    <t>TODO: Coverage of the Sequence Assembly. Only use this column if the Analysis is of type Sequence Assembly.</t>
+  </si>
+  <si>
+    <t>TODO: Platform used for the Sequence Assembly. Only use this column if the Analysis is of type Sequence Assembly.</t>
+  </si>
+  <si>
+    <t>TODO: Minimum Gap length used of the Sequence Assembly. Only use this column if the Analysis is of type Sequence Assembly.</t>
+  </si>
+  <si>
+    <t>TODO: Molecule type used in the Sequence Assembly. Only use this column if the Analysis is of type Sequence Assembly. Must be value from Controlled vocabulary:
+	genomic DNA
+	genomic RNA
+	viral cRNA</t>
+  </si>
+  <si>
+    <t>TODO: Program used for the Sequence Assembly. Only use this column if the Analysis is of type Sequence Assembly.</t>
+  </si>
+  <si>
+    <t>TODO: Specifies if the Sequence assembly is partial or not (use 'True' or 'False'). Only use this column if the Analysis is of type Sequence Assembly.</t>
+  </si>
+  <si>
+    <t>TODO: Program used for the Genome Mapping. Use this column exclusively if the Analysis is of type Genome Map.</t>
+  </si>
+  <si>
+    <t>TODO: Platform used for the Genome Mapping. Use this column exclusively if the Analysis is of type Genome Map.</t>
+  </si>
+  <si>
+    <t>TODO: Description of the Genome Map. Use this column exclusively if the Analysis is of type Genome Map.</t>
+  </si>
+  <si>
+    <t>TODO: Name of the transcriptome assembly. Use this column exclusively if the Analysis is of type Transcriptome Assembly.</t>
+  </si>
+  <si>
+    <t>TODO: Type of the transcriptome assembly. Use this column exclusively if the Analysis is of type Transcriptome Assembly. Must be value from Controlled vocabulary: 
+	isolate
+	metatranscriptome</t>
+  </si>
+  <si>
+    <t>TODO: Platform used for the transcriptome assembly. Use this column exclusively if the Analysis is of type Transcriptome Assembly.</t>
+  </si>
+  <si>
+    <t>TODO: Program used for the transcriptome assembly. Use this column exclusively if the Analysis is of type Transcriptome Assembly.</t>
+  </si>
+  <si>
+    <t>READ_SPEC.READ_LABEL</t>
+  </si>
+  <si>
+    <t>READ_SPEC.READ_INDEX</t>
+  </si>
+  <si>
+    <t>READ_SPEC.BASE_COORD</t>
+  </si>
+  <si>
+    <t>READ_SPEC.READ_CLASS</t>
+  </si>
+  <si>
+    <t>READ_SPEC.READ_TYPE</t>
+  </si>
+  <si>
+    <t>READ_SPEC.Preceding_read_index</t>
+  </si>
+  <si>
+    <t>READ_SPEC.Expected_Default_Length</t>
+  </si>
+  <si>
+    <t>READ_SPEC.Basecall</t>
+  </si>
+  <si>
+    <t>READ_SPEC.Basecall_min_match</t>
+  </si>
+  <si>
+    <t>READ_SPEC.Basecall_max_mismatch</t>
+  </si>
+  <si>
+    <t>READ_SPEC.Basecall_match_edge</t>
+  </si>
+  <si>
+    <t>TODO: the class of the read. Must be value from Controlled vocabulary: 'Application Read' or 'Technical Read'.</t>
+  </si>
+  <si>
+    <t>Read this overview before anything else!</t>
   </si>
   <si>
     <t>What is metadata?</t>
-  </si>
-  <si>
-    <t>What is this file?</t>
-  </si>
-  <si>
-    <t>This is a template spreadsheet (.xlsx) of metadata.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For what? </t>
-  </si>
-  <si>
-    <t>What are these tabs?</t>
-  </si>
-  <si>
-    <t>Each excel tab besides this one (Readme) represents a metadata object within the data model of the EGA. In other words, each tab will hold the information of one single metadata object (e.g. sample, study…)</t>
-  </si>
-  <si>
-    <t>You simply have to fill out the rows and columns of the tabs that are relevant to your submission (i.e. if you are only submitting samples' metadata, other tabs can be left empty). In each tab you will find a grey line at the third row, below which you shall enter your real metadata. In the begining, the template will contain a "mock" example at row 4 for you to visualise (contains things like "Example!_..."), remove it and use your real metadata there.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Ok, but </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>what do I do</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">? </t>
-    </r>
   </si>
   <si>
     <r>
@@ -1703,85 +1546,13 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Repeated columns? </t>
-  </si>
-  <si>
-    <t>Read this overview before anything else!</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Descriptive</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> row (explains what type of data corresponds to each column). Fields that do not start with "TODO:…" must contain the string that is left within this row. For instance, one of the TAG columns within the Sample tab is "phenotype", which means that this column shall contain "phenotype" for each and every row. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Real data</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (all rows from 4 onwards will be transformed into XML nodes by the star2xml tool)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Column headers that do not appear to be chosen for any metadata instance (row), and thus </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>can be ignored</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (i.e. left empty) (based on multiple choice attributes)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Within each tab, you will find a dark vertical line, beyond which there will be repeated "blocks" of columns. These blocks can be repeated indefinetely (i.e. add or remove as many of this blocks/columns as you need) but always as a complete block. See the column headers' format below. </t>
+    <t>What is this file?</t>
+  </si>
+  <si>
+    <t>This is a template spreadsheet (.xlsx) of metadata.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For what? </t>
   </si>
   <si>
     <r>
@@ -1851,6 +1622,47 @@
     </r>
   </si>
   <si>
+    <t>What are these tabs?</t>
+  </si>
+  <si>
+    <t>Each excel tab besides this one (Readme) represents a metadata object within the data model of the EGA. In other words, each tab will hold the information of one single metadata object (e.g. sample, study…)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ok, but </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>what do I do</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">? </t>
+    </r>
+  </si>
+  <si>
+    <t>You simply have to fill out the rows and columns of the tabs that are relevant to your submission (i.e. if you are only submitting samples' metadata, other tabs can be left empty). In each tab you will find a grey line at the third row, below which you shall enter your real metadata. In the begining, the template will contain a "mock" example at row 4 for you to visualise (contains things like "Example!_..."), remove it and use your real metadata there.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repeated columns? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Within each tab, you will find a dark vertical line, beyond which there will be repeated "blocks" of columns. These blocks can be repeated indefinetely (i.e. add or remove as many of this blocks/columns as you need) but always as a complete block. See the column headers' format below. </t>
+  </si>
+  <si>
     <r>
       <t>For further information, go to "</t>
     </r>
@@ -1874,6 +1686,87 @@
       </rPr>
       <t>", where additional information regarding the filling of this template can be found.</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descriptive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> row (explains what type of data corresponds to each column). Fields that do not start with "TODO:…" must contain the string that is left within this row. For instance, one of the TAG columns within the Sample tab is "phenotype", which means that this column shall contain "phenotype" for each and every row. </t>
+    </r>
+  </si>
+  <si>
+    <t>Real data "ceiling" (put your real data beneath this row)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Real data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (all rows from 4 onwards will be transformed into XML nodes by the star2xml tool)</t>
+    </r>
+  </si>
+  <si>
+    <t>Optional ( yet highly recommended) attributes</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Column headers that do not appear to be chosen for any metadata instance (row), and thus </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>can be ignored</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (i.e. left empty) (based on multiple choice attributes)</t>
+    </r>
+  </si>
+  <si>
+    <t>Repeated blocks (each with their own colour): you can add or remove as many "whole" blocks as you want to fulfil your needs, but remember to always work with complete repetitions (e.g. adding three new columns TAG-VALUE-UNITS for a new attribute, but not adding only one or two of them TAG-VALUE)</t>
   </si>
 </sst>
 </file>
@@ -1958,7 +1851,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2057,18 +1950,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFE9EDF7"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2097,19 +1978,40 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2C4E9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE0EED6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7DDF2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE5E5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
@@ -2230,6 +2132,17 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -2244,23 +2157,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2271,9 +2173,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2281,11 +2180,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2305,18 +2200,18 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2326,34 +2221,25 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2366,7 +2252,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2385,77 +2271,123 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="39">
+  <dxfs count="62">
     <dxf>
       <font>
         <strike val="0"/>
@@ -2517,48 +2449,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFB7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFB7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFB7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
       </font>
@@ -2599,6 +2489,66 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFFB7"/>
@@ -2623,6 +2573,218 @@
       <fill>
         <patternFill>
           <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFB7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFB7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFB7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2820,6 +2982,13 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFE5E5"/>
+      <color rgb="FFFF9999"/>
+      <color rgb="FFF7DDF2"/>
+      <color rgb="FFF2C4E9"/>
+      <color rgb="FFFFF5D5"/>
+      <color rgb="FFE0EED6"/>
+      <color rgb="FFD8EEC0"/>
       <color rgb="FFFFFFB7"/>
       <color rgb="FFCDACE6"/>
     </mruColors>
@@ -3101,7 +3270,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3112,90 +3281,90 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="87" t="s">
-        <v>398</v>
-      </c>
-      <c r="B2" s="86"/>
+      <c r="A2" s="95" t="s">
+        <v>385</v>
+      </c>
+      <c r="B2" s="96"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="83" t="s">
-        <v>388</v>
-      </c>
-      <c r="B3" s="82" t="s">
-        <v>396</v>
+      <c r="A3" s="75" t="s">
+        <v>386</v>
+      </c>
+      <c r="B3" s="69" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="75" t="s">
+        <v>388</v>
+      </c>
+      <c r="B4" s="69" t="s">
         <v>389</v>
-      </c>
-      <c r="B4" s="82" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="84" t="s">
+      <c r="A5" s="76" t="s">
+        <v>390</v>
+      </c>
+      <c r="B5" s="69" t="s">
         <v>391</v>
-      </c>
-      <c r="B5" s="82" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="84" t="s">
+      <c r="A6" s="76" t="s">
         <v>392</v>
       </c>
-      <c r="B6" s="82" t="s">
+      <c r="B6" s="69" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="76" t="s">
+        <v>394</v>
+      </c>
+      <c r="B7" s="69" t="s">
         <v>395</v>
-      </c>
-      <c r="B7" s="82" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="84" t="s">
+      <c r="A8" s="76" t="s">
+        <v>396</v>
+      </c>
+      <c r="B8" s="69" t="s">
         <v>397</v>
-      </c>
-      <c r="B8" s="82" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="88" t="s">
-        <v>404</v>
-      </c>
-      <c r="B9" s="88"/>
+      <c r="A9" s="97" t="s">
+        <v>398</v>
+      </c>
+      <c r="B9" s="97"/>
     </row>
     <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="85" t="s">
-        <v>119</v>
-      </c>
-      <c r="B11" s="86"/>
+      <c r="A11" s="98" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="96"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>121</v>
+      <c r="A12" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="32">
+      <c r="A13" s="28">
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="33">
+      <c r="A14" s="29">
         <v>2</v>
       </c>
       <c r="B14" t="s">
@@ -3203,85 +3372,84 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="33">
+      <c r="A15" s="29">
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>387</v>
+        <v>400</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
-        <v>123</v>
+      <c r="A16" s="30" t="s">
+        <v>111</v>
       </c>
       <c r="B16" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="85" t="s">
-        <v>124</v>
-      </c>
-      <c r="B18" s="86"/>
+      <c r="A18" s="98" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" s="96"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>121</v>
+      <c r="A19" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>127</v>
+      <c r="A20" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>385</v>
+      <c r="A21" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>144</v>
+      <c r="A22" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
-        <v>143</v>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>401</v>
+      <c r="A23" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="27" t="s">
-        <v>129</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>386</v>
+      <c r="A24" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>404</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A9:B9"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3301,17 +3469,17 @@
     <col min="4" max="4" width="12.140625" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="6" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" style="39" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" style="34" customWidth="1"/>
     <col min="11" max="12" width="8.7109375" style="2" customWidth="1"/>
     <col min="13" max="15" width="8.7109375" customWidth="1"/>
     <col min="16" max="18" width="8.7109375" style="2" customWidth="1"/>
-    <col min="19" max="22" width="10.85546875" style="50" customWidth="1"/>
+    <col min="19" max="22" width="10.85546875" style="44" customWidth="1"/>
     <col min="23" max="26" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -3320,24 +3488,24 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="E1" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="G1" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="H1" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="I1" t="s">
-        <v>151</v>
-      </c>
-      <c r="J1" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="J1" s="31" t="s">
         <v>0</v>
       </c>
       <c r="K1" s="4" t="s">
@@ -3364,224 +3532,225 @@
       <c r="R1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="36" t="s">
-        <v>152</v>
-      </c>
-      <c r="T1" s="36" t="s">
-        <v>153</v>
-      </c>
-      <c r="U1" s="36" t="s">
-        <v>154</v>
-      </c>
-      <c r="V1" s="36" t="s">
-        <v>155</v>
-      </c>
-      <c r="W1" s="36" t="s">
-        <v>152</v>
-      </c>
-      <c r="X1" s="36" t="s">
-        <v>153</v>
-      </c>
-      <c r="Y1" s="36" t="s">
-        <v>154</v>
-      </c>
-      <c r="Z1" s="36" t="s">
-        <v>155</v>
+      <c r="S1" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="T1" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="U1" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="V1" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="W1" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="X1" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y1" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z1" s="32" t="s">
+        <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E2" s="37" t="s">
-        <v>158</v>
-      </c>
-      <c r="F2" t="s">
-        <v>159</v>
-      </c>
-      <c r="G2" s="38" t="s">
-        <v>160</v>
-      </c>
-      <c r="H2" t="s">
-        <v>161</v>
-      </c>
-      <c r="I2" t="s">
-        <v>162</v>
+    <row r="2" spans="1:26" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>146</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="I2" s="38" t="s">
+        <v>150</v>
       </c>
       <c r="J2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="40" t="s">
+      <c r="S2" s="83" t="s">
+        <v>151</v>
+      </c>
+      <c r="T2" s="83" t="s">
+        <v>152</v>
+      </c>
+      <c r="U2" s="83" t="s">
+        <v>153</v>
+      </c>
+      <c r="V2" s="83" t="s">
+        <v>154</v>
+      </c>
+      <c r="W2" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="X2" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="Y2" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="Z2" s="33" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="M3" s="37"/>
+    </row>
+    <row r="4" spans="1:26" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="38" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="H4" s="38" t="s">
+        <v>159</v>
+      </c>
+      <c r="I4" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="J4" s="39" t="s">
+        <v>161</v>
+      </c>
+      <c r="K4" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="L4" s="40"/>
+      <c r="M4" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="T2" s="40" t="s">
+      <c r="N4" s="38" t="s">
         <v>164</v>
       </c>
-      <c r="U2" s="40" t="s">
+      <c r="P4" s="40" t="s">
         <v>165</v>
       </c>
-      <c r="V2" s="40" t="s">
+      <c r="Q4" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="R4" s="40"/>
+      <c r="S4" s="41" t="s">
         <v>166</v>
       </c>
-      <c r="W2" s="38" t="s">
-        <v>163</v>
-      </c>
-      <c r="X2" s="38" t="s">
-        <v>164</v>
-      </c>
-      <c r="Y2" s="38" t="s">
-        <v>165</v>
-      </c>
-      <c r="Z2" s="38" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
-        <v>118</v>
-      </c>
-      <c r="M3" s="43"/>
-    </row>
-    <row r="4" spans="1:26" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
+      <c r="T4" s="41">
+        <v>406</v>
+      </c>
+      <c r="U4" s="41" t="s">
         <v>167</v>
       </c>
-      <c r="B4" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="44" t="s">
+      <c r="V4" s="42" t="s">
         <v>168</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="W4" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="G4" s="37" t="s">
+      <c r="X4" s="38">
+        <v>110649</v>
+      </c>
+      <c r="Y4" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="H4" s="44" t="s">
+      <c r="Z4" s="43" t="s">
         <v>171</v>
-      </c>
-      <c r="I4" s="44" t="s">
-        <v>172</v>
-      </c>
-      <c r="J4" s="45" t="s">
-        <v>173</v>
-      </c>
-      <c r="K4" s="46" t="s">
-        <v>174</v>
-      </c>
-      <c r="L4" s="46"/>
-      <c r="M4" s="44" t="s">
-        <v>175</v>
-      </c>
-      <c r="N4" s="44" t="s">
-        <v>176</v>
-      </c>
-      <c r="P4" s="46" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q4" s="46" t="s">
-        <v>174</v>
-      </c>
-      <c r="R4" s="46"/>
-      <c r="S4" s="47" t="s">
-        <v>178</v>
-      </c>
-      <c r="T4" s="47">
-        <v>406</v>
-      </c>
-      <c r="U4" s="47" t="s">
-        <v>179</v>
-      </c>
-      <c r="V4" s="48" t="s">
-        <v>180</v>
-      </c>
-      <c r="W4" s="44" t="s">
-        <v>181</v>
-      </c>
-      <c r="X4" s="44">
-        <v>110649</v>
-      </c>
-      <c r="Y4" s="44" t="s">
-        <v>182</v>
-      </c>
-      <c r="Z4" s="49" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="P7" s="46"/>
-      <c r="Q7" s="46"/>
-      <c r="R7" s="46"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:I1 K1:L1 T1:V1 AA1:XFD1">
-    <cfRule type="containsText" dxfId="38" priority="6" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="61" priority="12" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1">
-    <cfRule type="containsText" dxfId="37" priority="5" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="60" priority="11" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",S1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X1:Z1">
-    <cfRule type="containsText" dxfId="36" priority="4" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="59" priority="10" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",X1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W1">
-    <cfRule type="containsText" dxfId="35" priority="3" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="58" priority="9" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",W1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:O1">
-    <cfRule type="containsText" dxfId="34" priority="2" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="57" priority="8" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",N1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:R1">
-    <cfRule type="containsText" dxfId="33" priority="1" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="56" priority="7" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",Q1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3612,7 +3781,7 @@
     <col min="15" max="15" width="10.140625" style="2" customWidth="1"/>
     <col min="16" max="16" width="6.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6.140625" style="2" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="6.42578125" style="39" customWidth="1"/>
+    <col min="18" max="18" width="6.42578125" style="34" customWidth="1"/>
     <col min="19" max="19" width="6.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7.28515625" style="2" customWidth="1"/>
     <col min="21" max="21" width="6.42578125" customWidth="1"/>
@@ -3625,7 +3794,7 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>313</v>
+        <v>284</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -3634,48 +3803,48 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>314</v>
+        <v>285</v>
       </c>
       <c r="E1" t="s">
-        <v>315</v>
+        <v>286</v>
       </c>
       <c r="F1" t="s">
-        <v>316</v>
+        <v>287</v>
       </c>
       <c r="G1" t="s">
-        <v>317</v>
+        <v>288</v>
       </c>
       <c r="H1" t="s">
-        <v>121</v>
-      </c>
-      <c r="I1" s="69" t="s">
+        <v>109</v>
+      </c>
+      <c r="I1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="70" t="s">
+      <c r="J1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="71" t="s">
+      <c r="K1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="72" t="s">
+      <c r="L1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="73" t="s">
+      <c r="M1" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="74" t="s">
+      <c r="N1" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="69" t="s">
+      <c r="O1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="P1" s="70" t="s">
+      <c r="P1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="70" t="s">
+      <c r="Q1" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="35" t="s">
+      <c r="R1" s="31" t="s">
         <v>0</v>
       </c>
       <c r="S1" s="4" t="s">
@@ -3703,90 +3872,90 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="44" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
-        <v>318</v>
-      </c>
-      <c r="B2" s="44" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="44" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" s="44" t="s">
-        <v>319</v>
-      </c>
-      <c r="E2" s="44" t="s">
-        <v>320</v>
-      </c>
-      <c r="F2" s="44" t="s">
-        <v>321</v>
-      </c>
-      <c r="G2" s="44" t="s">
-        <v>322</v>
-      </c>
-      <c r="H2" s="44" t="s">
-        <v>323</v>
-      </c>
-      <c r="I2" s="46" t="s">
-        <v>324</v>
-      </c>
-      <c r="J2" s="46" t="s">
-        <v>325</v>
-      </c>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46" t="s">
-        <v>326</v>
-      </c>
-      <c r="M2" s="75" t="s">
-        <v>327</v>
-      </c>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46" t="s">
-        <v>328</v>
-      </c>
-      <c r="P2" s="46" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="45" t="s">
-        <v>330</v>
-      </c>
-      <c r="S2" s="46" t="s">
-        <v>331</v>
-      </c>
-      <c r="T2" s="46" t="s">
-        <v>332</v>
-      </c>
-      <c r="U2" s="44" t="s">
-        <v>330</v>
-      </c>
-      <c r="V2" s="44" t="s">
-        <v>331</v>
-      </c>
-      <c r="W2" s="44" t="s">
-        <v>332</v>
-      </c>
-      <c r="X2" s="46" t="s">
-        <v>330</v>
-      </c>
-      <c r="Y2" s="46" t="s">
-        <v>331</v>
-      </c>
-      <c r="Z2" s="46" t="s">
-        <v>332</v>
+    <row r="2" spans="1:26" s="38" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>289</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>290</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>291</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>292</v>
+      </c>
+      <c r="G2" s="38" t="s">
+        <v>293</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>294</v>
+      </c>
+      <c r="I2" s="40" t="s">
+        <v>295</v>
+      </c>
+      <c r="J2" s="40" t="s">
+        <v>296</v>
+      </c>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40" t="s">
+        <v>297</v>
+      </c>
+      <c r="M2" s="63" t="s">
+        <v>298</v>
+      </c>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40" t="s">
+        <v>299</v>
+      </c>
+      <c r="P2" s="40" t="s">
+        <v>300</v>
+      </c>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="39" t="s">
+        <v>301</v>
+      </c>
+      <c r="S2" s="40" t="s">
+        <v>302</v>
+      </c>
+      <c r="T2" s="40" t="s">
+        <v>303</v>
+      </c>
+      <c r="U2" s="38" t="s">
+        <v>301</v>
+      </c>
+      <c r="V2" s="38" t="s">
+        <v>302</v>
+      </c>
+      <c r="W2" s="38" t="s">
+        <v>303</v>
+      </c>
+      <c r="X2" s="40" t="s">
+        <v>301</v>
+      </c>
+      <c r="Y2" s="40" t="s">
+        <v>302</v>
+      </c>
+      <c r="Z2" s="40" t="s">
+        <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="20" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="M3" s="21"/>
-      <c r="R3" s="76"/>
+    <row r="3" spans="1:26" s="17" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="M3" s="18"/>
+      <c r="R3" s="64"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>333</v>
+        <v>304</v>
       </c>
       <c r="B4" t="s">
         <v>43</v>
@@ -3795,76 +3964,76 @@
         <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>334</v>
+        <v>305</v>
       </c>
       <c r="E4">
         <v>9606</v>
       </c>
       <c r="F4" t="s">
-        <v>335</v>
+        <v>306</v>
       </c>
       <c r="G4" t="s">
-        <v>336</v>
+        <v>307</v>
       </c>
       <c r="H4" t="s">
-        <v>337</v>
+        <v>308</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>324</v>
+        <v>295</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>305</v>
+        <v>276</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>326</v>
+        <v>297</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>338</v>
+        <v>309</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>328</v>
+        <v>299</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="R4" s="39" t="s">
-        <v>340</v>
+        <v>310</v>
+      </c>
+      <c r="R4" s="34" t="s">
+        <v>311</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>341</v>
+        <v>312</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>342</v>
+        <v>313</v>
       </c>
       <c r="U4" t="s">
-        <v>343</v>
+        <v>314</v>
       </c>
       <c r="V4" t="s">
-        <v>344</v>
+        <v>315</v>
       </c>
       <c r="W4" t="s">
-        <v>342</v>
+        <v>313</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>345</v>
+        <v>316</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>346</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:T1 AA1:XFD1">
-    <cfRule type="containsText" dxfId="32" priority="3" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="50" priority="11" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:W1">
-    <cfRule type="containsText" dxfId="31" priority="2" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="49" priority="10" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",U1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X1:Z1">
-    <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="48" priority="9" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",X1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3890,22 +4059,24 @@
     <col min="6" max="6" width="15.5703125" customWidth="1"/>
     <col min="7" max="7" width="20.28515625" customWidth="1"/>
     <col min="8" max="29" width="15.5703125" customWidth="1"/>
-    <col min="30" max="30" width="8.7109375" style="59" customWidth="1"/>
+    <col min="30" max="30" width="8.7109375" style="34" customWidth="1"/>
     <col min="31" max="32" width="8.7109375" style="2" customWidth="1"/>
-    <col min="33" max="34" width="15.5703125" style="67" customWidth="1"/>
+    <col min="33" max="34" width="15.5703125" style="55" customWidth="1"/>
     <col min="35" max="36" width="15.5703125" customWidth="1"/>
-    <col min="37" max="38" width="15.5703125" style="67" customWidth="1"/>
-    <col min="39" max="44" width="8.7109375" style="61" customWidth="1"/>
+    <col min="37" max="38" width="15.5703125" style="55" customWidth="1"/>
+    <col min="39" max="44" width="8.7109375" style="50" customWidth="1"/>
     <col min="45" max="50" width="8.7109375" customWidth="1"/>
-    <col min="51" max="52" width="8.7109375" style="63" customWidth="1"/>
+    <col min="51" max="52" width="8.7109375" style="51" customWidth="1"/>
     <col min="53" max="54" width="8.7109375" customWidth="1"/>
-    <col min="55" max="56" width="8.7109375" style="63" customWidth="1"/>
-    <col min="57" max="61" width="8.7109375" customWidth="1"/>
+    <col min="55" max="56" width="8.7109375" style="51" customWidth="1"/>
+    <col min="57" max="58" width="8.7109375" style="71" customWidth="1"/>
+    <col min="59" max="60" width="8.7109375" style="93" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="8.7109375" style="72" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:61" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -3914,84 +4085,84 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="E1" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="F1" t="s">
         <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="H1" t="s">
+        <v>175</v>
+      </c>
+      <c r="I1" t="s">
+        <v>176</v>
+      </c>
+      <c r="J1" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="K1" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="L1" s="45" t="s">
+        <v>179</v>
+      </c>
+      <c r="M1" s="45" t="s">
+        <v>180</v>
+      </c>
+      <c r="N1" s="45" t="s">
+        <v>181</v>
+      </c>
+      <c r="O1" s="45" t="s">
+        <v>182</v>
+      </c>
+      <c r="P1" s="45" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q1" s="45" t="s">
+        <v>184</v>
+      </c>
+      <c r="R1" s="45" t="s">
+        <v>185</v>
+      </c>
+      <c r="S1" s="45" t="s">
+        <v>186</v>
+      </c>
+      <c r="T1" s="45" t="s">
         <v>187</v>
       </c>
-      <c r="I1" t="s">
+      <c r="U1" s="45" t="s">
         <v>188</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="V1" s="45" t="s">
         <v>189</v>
       </c>
-      <c r="K1" s="51" t="s">
+      <c r="W1" s="45" t="s">
         <v>190</v>
       </c>
-      <c r="L1" s="51" t="s">
+      <c r="X1" s="45" t="s">
         <v>191</v>
       </c>
-      <c r="M1" s="51" t="s">
+      <c r="Y1" s="45" t="s">
         <v>192</v>
       </c>
-      <c r="N1" s="51" t="s">
+      <c r="Z1" s="45" t="s">
         <v>193</v>
       </c>
-      <c r="O1" s="51" t="s">
+      <c r="AA1" s="45" t="s">
         <v>194</v>
       </c>
-      <c r="P1" s="51" t="s">
+      <c r="AB1" s="45" t="s">
         <v>195</v>
       </c>
-      <c r="Q1" s="51" t="s">
+      <c r="AC1" s="45" t="s">
         <v>196</v>
       </c>
-      <c r="R1" s="51" t="s">
-        <v>197</v>
-      </c>
-      <c r="S1" s="51" t="s">
-        <v>198</v>
-      </c>
-      <c r="T1" s="51" t="s">
-        <v>199</v>
-      </c>
-      <c r="U1" s="51" t="s">
-        <v>200</v>
-      </c>
-      <c r="V1" s="51" t="s">
-        <v>201</v>
-      </c>
-      <c r="W1" s="51" t="s">
-        <v>202</v>
-      </c>
-      <c r="X1" s="51" t="s">
-        <v>203</v>
-      </c>
-      <c r="Y1" s="51" t="s">
-        <v>204</v>
-      </c>
-      <c r="Z1" s="51" t="s">
-        <v>205</v>
-      </c>
-      <c r="AA1" s="51" t="s">
-        <v>206</v>
-      </c>
-      <c r="AB1" s="51" t="s">
-        <v>207</v>
-      </c>
-      <c r="AC1" s="51" t="s">
-        <v>208</v>
-      </c>
-      <c r="AD1" s="52" t="s">
+      <c r="AD1" s="31" t="s">
         <v>0</v>
       </c>
       <c r="AE1" s="4" t="s">
@@ -4000,288 +4171,291 @@
       <c r="AF1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AG1" s="53" t="s">
+      <c r="AG1" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="AH1" s="46" t="s">
+        <v>198</v>
+      </c>
+      <c r="AI1" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="AJ1" s="46" t="s">
+        <v>198</v>
+      </c>
+      <c r="AK1" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="AL1" s="46" t="s">
+        <v>198</v>
+      </c>
+      <c r="AM1" s="47" t="s">
+        <v>199</v>
+      </c>
+      <c r="AN1" s="47" t="s">
+        <v>200</v>
+      </c>
+      <c r="AO1" s="47" t="s">
+        <v>201</v>
+      </c>
+      <c r="AP1" s="47" t="s">
+        <v>202</v>
+      </c>
+      <c r="AQ1" s="47" t="s">
+        <v>203</v>
+      </c>
+      <c r="AR1" s="47" t="s">
+        <v>204</v>
+      </c>
+      <c r="AS1" s="47" t="s">
+        <v>199</v>
+      </c>
+      <c r="AT1" s="47" t="s">
+        <v>200</v>
+      </c>
+      <c r="AU1" s="47" t="s">
+        <v>201</v>
+      </c>
+      <c r="AV1" s="47" t="s">
+        <v>202</v>
+      </c>
+      <c r="AW1" s="47" t="s">
+        <v>203</v>
+      </c>
+      <c r="AX1" s="47" t="s">
+        <v>204</v>
+      </c>
+      <c r="AY1" s="48" t="s">
+        <v>205</v>
+      </c>
+      <c r="AZ1" s="48" t="s">
+        <v>206</v>
+      </c>
+      <c r="BA1" s="48" t="s">
+        <v>205</v>
+      </c>
+      <c r="BB1" s="48" t="s">
+        <v>206</v>
+      </c>
+      <c r="BC1" s="48" t="s">
+        <v>205</v>
+      </c>
+      <c r="BD1" s="48" t="s">
+        <v>206</v>
+      </c>
+      <c r="BE1" s="49" t="s">
+        <v>207</v>
+      </c>
+      <c r="BF1" s="49" t="s">
+        <v>208</v>
+      </c>
+      <c r="BG1" s="92" t="s">
         <v>209</v>
       </c>
-      <c r="AH1" s="53" t="s">
+      <c r="BH1" s="92" t="s">
         <v>210</v>
       </c>
-      <c r="AI1" s="53" t="s">
-        <v>209</v>
-      </c>
-      <c r="AJ1" s="53" t="s">
-        <v>210</v>
-      </c>
-      <c r="AK1" s="53" t="s">
-        <v>209</v>
-      </c>
-      <c r="AL1" s="53" t="s">
-        <v>210</v>
-      </c>
-      <c r="AM1" s="54" t="s">
+      <c r="BI1" s="70" t="s">
         <v>211</v>
       </c>
-      <c r="AN1" s="54" t="s">
+    </row>
+    <row r="2" spans="1:61" s="38" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
         <v>212</v>
       </c>
-      <c r="AO1" s="54" t="s">
+      <c r="B2" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="AP1" s="54" t="s">
+      <c r="E2" s="33" t="s">
         <v>214</v>
       </c>
-      <c r="AQ1" s="54" t="s">
+      <c r="F2" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="AR1" s="54" t="s">
+      <c r="G2" s="33" t="s">
         <v>216</v>
       </c>
-      <c r="AS1" s="54" t="s">
-        <v>211</v>
-      </c>
-      <c r="AT1" s="54" t="s">
-        <v>212</v>
-      </c>
-      <c r="AU1" s="54" t="s">
-        <v>213</v>
-      </c>
-      <c r="AV1" s="54" t="s">
-        <v>214</v>
-      </c>
-      <c r="AW1" s="54" t="s">
-        <v>215</v>
-      </c>
-      <c r="AX1" s="54" t="s">
-        <v>216</v>
-      </c>
-      <c r="AY1" s="55" t="s">
+      <c r="H2" s="38" t="s">
         <v>217</v>
       </c>
-      <c r="AZ1" s="55" t="s">
+      <c r="I2" s="33" t="s">
         <v>218</v>
       </c>
-      <c r="BA1" s="55" t="s">
-        <v>217</v>
-      </c>
-      <c r="BB1" s="55" t="s">
-        <v>218</v>
-      </c>
-      <c r="BC1" s="55" t="s">
-        <v>217</v>
-      </c>
-      <c r="BD1" s="55" t="s">
-        <v>218</v>
-      </c>
-      <c r="BE1" s="56" t="s">
+      <c r="J2" s="33" t="s">
         <v>219</v>
       </c>
-      <c r="BF1" s="56" t="s">
+      <c r="K2" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="BG1" s="57" t="s">
+      <c r="L2" s="33" t="s">
         <v>221</v>
       </c>
-      <c r="BH1" s="57" t="s">
+      <c r="M2" s="38" t="s">
+        <v>356</v>
+      </c>
+      <c r="N2" s="38" t="s">
+        <v>357</v>
+      </c>
+      <c r="O2" s="38" t="s">
+        <v>358</v>
+      </c>
+      <c r="P2" s="33" t="s">
+        <v>359</v>
+      </c>
+      <c r="Q2" s="38" t="s">
+        <v>360</v>
+      </c>
+      <c r="R2" s="38" t="s">
+        <v>361</v>
+      </c>
+      <c r="S2" s="38" t="s">
+        <v>362</v>
+      </c>
+      <c r="T2" s="33" t="s">
+        <v>363</v>
+      </c>
+      <c r="U2" s="38" t="s">
+        <v>364</v>
+      </c>
+      <c r="V2" s="38" t="s">
+        <v>365</v>
+      </c>
+      <c r="W2" s="38" t="s">
+        <v>366</v>
+      </c>
+      <c r="X2" s="38" t="s">
+        <v>367</v>
+      </c>
+      <c r="Y2" s="38" t="s">
+        <v>368</v>
+      </c>
+      <c r="Z2" s="38" t="s">
+        <v>369</v>
+      </c>
+      <c r="AA2" s="33" t="s">
+        <v>370</v>
+      </c>
+      <c r="AB2" s="38" t="s">
+        <v>371</v>
+      </c>
+      <c r="AC2" s="38" t="s">
+        <v>372</v>
+      </c>
+      <c r="AD2" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE2" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF2" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG2" s="77" t="s">
         <v>222</v>
       </c>
-      <c r="BI1" s="58" t="s">
+      <c r="AH2" s="77" t="s">
         <v>223</v>
       </c>
+      <c r="AI2" s="33" t="s">
+        <v>222</v>
+      </c>
+      <c r="AJ2" s="33" t="s">
+        <v>223</v>
+      </c>
+      <c r="AK2" s="77" t="s">
+        <v>222</v>
+      </c>
+      <c r="AL2" s="77" t="s">
+        <v>223</v>
+      </c>
+      <c r="AM2" s="78" t="s">
+        <v>224</v>
+      </c>
+      <c r="AN2" s="79" t="s">
+        <v>225</v>
+      </c>
+      <c r="AO2" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="AP2" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="AQ2" s="78" t="s">
+        <v>228</v>
+      </c>
+      <c r="AR2" s="78" t="s">
+        <v>229</v>
+      </c>
+      <c r="AS2" s="38" t="s">
+        <v>224</v>
+      </c>
+      <c r="AT2" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="AU2" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="AV2" s="38" t="s">
+        <v>227</v>
+      </c>
+      <c r="AW2" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="AX2" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="AY2" s="80" t="s">
+        <v>231</v>
+      </c>
+      <c r="AZ2" s="80" t="s">
+        <v>232</v>
+      </c>
+      <c r="BA2" s="38" t="s">
+        <v>231</v>
+      </c>
+      <c r="BB2" s="38" t="s">
+        <v>232</v>
+      </c>
+      <c r="BC2" s="80" t="s">
+        <v>231</v>
+      </c>
+      <c r="BD2" s="80" t="s">
+        <v>232</v>
+      </c>
+      <c r="BE2" s="81" t="s">
+        <v>233</v>
+      </c>
+      <c r="BF2" s="81" t="s">
+        <v>234</v>
+      </c>
+      <c r="BG2" s="94" t="s">
+        <v>235</v>
+      </c>
+      <c r="BH2" s="94" t="s">
+        <v>236</v>
+      </c>
+      <c r="BI2" s="82" t="s">
+        <v>237</v>
+      </c>
     </row>
-    <row r="2" spans="1:61" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" t="s">
-        <v>225</v>
-      </c>
-      <c r="E2" s="37" t="s">
-        <v>226</v>
-      </c>
-      <c r="F2" t="s">
-        <v>227</v>
-      </c>
-      <c r="G2" s="37" t="s">
-        <v>228</v>
-      </c>
-      <c r="H2" t="s">
-        <v>229</v>
-      </c>
-      <c r="I2" s="37" t="s">
-        <v>230</v>
-      </c>
-      <c r="J2" s="37" t="s">
-        <v>231</v>
-      </c>
-      <c r="K2" s="37" t="s">
-        <v>232</v>
-      </c>
-      <c r="L2" s="38" t="s">
-        <v>233</v>
-      </c>
-      <c r="M2" t="s">
-        <v>234</v>
-      </c>
-      <c r="N2" t="s">
-        <v>235</v>
-      </c>
-      <c r="O2" t="s">
-        <v>236</v>
-      </c>
-      <c r="P2" s="38" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>238</v>
-      </c>
-      <c r="R2" t="s">
-        <v>239</v>
-      </c>
-      <c r="S2" t="s">
-        <v>240</v>
-      </c>
-      <c r="T2" s="38" t="s">
-        <v>241</v>
-      </c>
-      <c r="U2" t="s">
-        <v>242</v>
-      </c>
-      <c r="V2" t="s">
-        <v>243</v>
-      </c>
-      <c r="W2" t="s">
-        <v>244</v>
-      </c>
-      <c r="X2" t="s">
-        <v>245</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>246</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>247</v>
-      </c>
-      <c r="AA2" s="38" t="s">
-        <v>248</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>249</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>250</v>
-      </c>
-      <c r="AD2" s="59" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AG2" s="60" t="s">
-        <v>251</v>
-      </c>
-      <c r="AH2" s="60" t="s">
-        <v>252</v>
-      </c>
-      <c r="AI2" s="38" t="s">
-        <v>251</v>
-      </c>
-      <c r="AJ2" s="38" t="s">
-        <v>252</v>
-      </c>
-      <c r="AK2" s="60" t="s">
-        <v>251</v>
-      </c>
-      <c r="AL2" s="60" t="s">
-        <v>252</v>
-      </c>
-      <c r="AM2" s="61" t="s">
-        <v>253</v>
-      </c>
-      <c r="AN2" s="62" t="s">
-        <v>254</v>
-      </c>
-      <c r="AO2" s="61" t="s">
-        <v>255</v>
-      </c>
-      <c r="AP2" s="61" t="s">
-        <v>256</v>
-      </c>
-      <c r="AQ2" s="61" t="s">
-        <v>257</v>
-      </c>
-      <c r="AR2" s="61" t="s">
-        <v>258</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>253</v>
-      </c>
-      <c r="AT2" s="38" t="s">
-        <v>259</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>255</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>256</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>257</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>258</v>
-      </c>
-      <c r="AY2" s="63" t="s">
-        <v>260</v>
-      </c>
-      <c r="AZ2" s="63" t="s">
-        <v>261</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>260</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>261</v>
-      </c>
-      <c r="BC2" s="63" t="s">
-        <v>260</v>
-      </c>
-      <c r="BD2" s="63" t="s">
-        <v>261</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>262</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>263</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>264</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>265</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="3" spans="1:61" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="L3" s="21"/>
+    <row r="3" spans="1:61" s="17" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="L3" s="18"/>
+      <c r="AD3" s="64"/>
+      <c r="BG3" s="36"/>
+      <c r="BH3" s="36"/>
     </row>
     <row r="4" spans="1:61" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>267</v>
+        <v>238</v>
       </c>
       <c r="B4" t="s">
         <v>43</v>
@@ -4290,233 +4464,228 @@
         <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>268</v>
+        <v>239</v>
       </c>
       <c r="E4" t="s">
         <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>269</v>
+        <v>240</v>
       </c>
       <c r="G4" t="s">
-        <v>270</v>
+        <v>241</v>
       </c>
       <c r="H4" t="s">
         <v>42</v>
       </c>
       <c r="I4" t="s">
-        <v>271</v>
+        <v>242</v>
       </c>
       <c r="J4" t="s">
-        <v>272</v>
+        <v>243</v>
       </c>
       <c r="K4" t="s">
-        <v>273</v>
+        <v>244</v>
       </c>
       <c r="L4" t="s">
-        <v>274</v>
+        <v>245</v>
       </c>
       <c r="M4" t="s">
-        <v>275</v>
+        <v>246</v>
       </c>
       <c r="N4" t="s">
-        <v>276</v>
+        <v>247</v>
       </c>
       <c r="O4" t="s">
-        <v>277</v>
+        <v>248</v>
       </c>
       <c r="P4" t="s">
-        <v>278</v>
+        <v>249</v>
       </c>
       <c r="Q4">
         <v>80</v>
       </c>
       <c r="R4" t="s">
-        <v>279</v>
+        <v>250</v>
       </c>
       <c r="S4">
         <v>10</v>
       </c>
       <c r="T4" t="s">
+        <v>251</v>
+      </c>
+      <c r="U4" t="s">
+        <v>252</v>
+      </c>
+      <c r="V4" s="52" t="s">
+        <v>171</v>
+      </c>
+      <c r="W4" s="53" t="s">
+        <v>253</v>
+      </c>
+      <c r="X4" t="s">
+        <v>254</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>255</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>256</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>257</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>258</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>259</v>
+      </c>
+      <c r="AD4" s="34" t="s">
+        <v>260</v>
+      </c>
+      <c r="AE4" s="54" t="s">
+        <v>261</v>
+      </c>
+      <c r="AG4" s="55" t="s">
+        <v>262</v>
+      </c>
+      <c r="AH4" s="55" t="s">
+        <v>263</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>264</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>265</v>
+      </c>
+      <c r="AK4" s="55" t="s">
+        <v>266</v>
+      </c>
+      <c r="AL4" s="55" t="s">
+        <v>267</v>
+      </c>
+      <c r="AM4" s="50" t="s">
+        <v>268</v>
+      </c>
+      <c r="AN4" s="50" t="s">
+        <v>269</v>
+      </c>
+      <c r="AO4" s="50" t="s">
+        <v>226</v>
+      </c>
+      <c r="AP4" s="50" t="s">
+        <v>270</v>
+      </c>
+      <c r="AQ4" s="50" t="s">
+        <v>271</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>272</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>273</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>226</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>274</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>275</v>
+      </c>
+      <c r="AY4" s="51" t="s">
+        <v>276</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>277</v>
+      </c>
+      <c r="BB4" t="s">
+        <v>278</v>
+      </c>
+      <c r="BC4" s="51" t="s">
+        <v>279</v>
+      </c>
+      <c r="BE4" s="71" t="s">
         <v>280</v>
       </c>
-      <c r="U4" t="s">
+      <c r="BG4" s="93" t="s">
         <v>281</v>
       </c>
-      <c r="V4" s="64" t="s">
-        <v>183</v>
-      </c>
-      <c r="W4" s="65" t="s">
+      <c r="BH4" s="93" t="s">
         <v>282</v>
       </c>
-      <c r="X4" t="s">
+      <c r="BI4" s="72" t="s">
         <v>283</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>284</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>285</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>286</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>287</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>288</v>
-      </c>
-      <c r="AD4" s="59" t="s">
-        <v>289</v>
-      </c>
-      <c r="AE4" s="66" t="s">
-        <v>290</v>
-      </c>
-      <c r="AG4" s="67" t="s">
-        <v>291</v>
-      </c>
-      <c r="AH4" s="67" t="s">
-        <v>292</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>293</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>294</v>
-      </c>
-      <c r="AK4" s="67" t="s">
-        <v>295</v>
-      </c>
-      <c r="AL4" s="67" t="s">
-        <v>296</v>
-      </c>
-      <c r="AM4" s="61" t="s">
-        <v>297</v>
-      </c>
-      <c r="AN4" s="61" t="s">
-        <v>298</v>
-      </c>
-      <c r="AO4" s="61" t="s">
-        <v>255</v>
-      </c>
-      <c r="AP4" s="61" t="s">
-        <v>299</v>
-      </c>
-      <c r="AQ4" s="61" t="s">
-        <v>300</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>301</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>302</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>255</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>303</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>304</v>
-      </c>
-      <c r="AY4" s="63" t="s">
-        <v>305</v>
-      </c>
-      <c r="BA4" t="s">
-        <v>306</v>
-      </c>
-      <c r="BB4" t="s">
-        <v>307</v>
-      </c>
-      <c r="BC4" s="63" t="s">
-        <v>308</v>
-      </c>
-      <c r="BE4" t="s">
-        <v>309</v>
-      </c>
-      <c r="BG4" t="s">
-        <v>310</v>
-      </c>
-      <c r="BH4" t="s">
-        <v>311</v>
-      </c>
-      <c r="BI4" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="17" spans="6:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F17" s="68"/>
+      <c r="F17" s="56"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:F1 AE1:AF1 AM1:AR1 BI1:XFD1 AY1:AZ1 H1:I1 M1:AC1">
-    <cfRule type="containsText" dxfId="29" priority="14" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="43" priority="20" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE1:BF1">
-    <cfRule type="containsText" dxfId="28" priority="13" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="42" priority="19" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",BE1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BG1:BH1">
-    <cfRule type="containsText" dxfId="27" priority="12" operator="containsText" text="~*">
-      <formula>NOT(ISERROR(SEARCH("~*",BG1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AG1:AH1">
-    <cfRule type="containsText" dxfId="26" priority="11" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="41" priority="17" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",AG1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA1:BB1">
-    <cfRule type="containsText" dxfId="25" priority="10" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="40" priority="16" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",BA1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC1:BD1">
-    <cfRule type="containsText" dxfId="24" priority="9" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="39" priority="15" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",BC1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS1:AX1">
-    <cfRule type="containsText" dxfId="23" priority="8" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="38" priority="14" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",AS1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="containsText" dxfId="22" priority="7" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="37" priority="13" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI1:AJ1">
-    <cfRule type="containsText" dxfId="21" priority="6" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="36" priority="12" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",AI1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK1:AL1">
-    <cfRule type="containsText" dxfId="20" priority="5" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="35" priority="11" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",AK1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:AC1">
-    <cfRule type="expression" dxfId="19" priority="3">
+    <cfRule type="expression" dxfId="34" priority="9">
       <formula>IF(COUNTIF($I$4:$I$1048576,"*"&amp;LEFT(L$1, FIND(".", L$1)-1)&amp;"*"),"FALSE","TRUE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:AC1">
-    <cfRule type="expression" dxfId="18" priority="4">
+    <cfRule type="expression" dxfId="33" priority="10">
       <formula>IF(COUNTIF($I$4:$I$1048576,"*"&amp;LEFT(L$1, FIND(".", L$1)-1)&amp;"*"),"TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:K1">
-    <cfRule type="expression" dxfId="17" priority="2">
+    <cfRule type="expression" dxfId="32" priority="8">
       <formula>IF(COUNTIF($I$4:$I$1048576,"*REFERENCE_ALIGNMENT*") + COUNTIF($I$4:$I$1048576,"*SEQUENCE_VARIATION*") + COUNTIF($I$4:$I$1048576,"*PROCESSED_READS*") + COUNTIF($I$4:$I$1048576,"*SEQUENCE_ANNOTATION*"),"FALSE","TRUE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:K1">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="31" priority="7">
       <formula>IF(COUNTIF($I$4:$I$1048576,"*REFERENCE_ALIGNMENT*") + COUNTIF($I$4:$I$1048576,"*SEQUENCE_VARIATION*") + COUNTIF($I$4:$I$1048576,"*PROCESSED_READS*") + COUNTIF($I$4:$I$1048576,"*SEQUENCE_ANNOTATION*"),"TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4543,16 +4712,16 @@
     <col min="3" max="3" width="13" style="1" customWidth="1"/>
     <col min="4" max="12" width="15.5703125" style="1" customWidth="1"/>
     <col min="13" max="13" width="19" style="1" customWidth="1"/>
-    <col min="14" max="14" width="21.7109375" style="8" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" style="8" customWidth="1"/>
-    <col min="16" max="19" width="15.5703125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" style="7" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" style="7" customWidth="1"/>
+    <col min="16" max="19" width="15.5703125" style="8" customWidth="1"/>
     <col min="20" max="31" width="15.5703125" style="1" customWidth="1"/>
-    <col min="32" max="32" width="8.7109375" style="12" customWidth="1"/>
-    <col min="33" max="42" width="8.7109375" style="13" customWidth="1"/>
-    <col min="43" max="47" width="8.7109375" style="16" customWidth="1"/>
-    <col min="48" max="52" width="8.7109375" style="10" customWidth="1"/>
+    <col min="32" max="32" width="8.7109375" style="74" customWidth="1"/>
+    <col min="33" max="42" width="8.7109375" style="11" customWidth="1"/>
+    <col min="43" max="47" width="8.7109375" style="13" customWidth="1"/>
+    <col min="48" max="52" width="8.7109375" style="9" customWidth="1"/>
     <col min="53" max="55" width="8.7109375" style="3" customWidth="1"/>
-    <col min="56" max="56" width="9.140625" style="11"/>
+    <col min="56" max="56" width="9.140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:58" x14ac:dyDescent="0.25">
@@ -4580,38 +4749,38 @@
       <c r="H1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="8" t="s">
-        <v>133</v>
+      <c r="M1" s="7" t="s">
+        <v>121</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="P1" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="S1" s="9" t="s">
-        <v>130</v>
+      <c r="S1" s="8" t="s">
+        <v>118</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>9</v>
@@ -4649,68 +4818,68 @@
       <c r="AE1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AF1" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG1" s="15" t="s">
+      <c r="AF1" s="73" t="s">
+        <v>373</v>
+      </c>
+      <c r="AG1" s="12" t="s">
+        <v>374</v>
+      </c>
+      <c r="AH1" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="AI1" s="12" t="s">
+        <v>376</v>
+      </c>
+      <c r="AJ1" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="AK1" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="AL1" s="12" t="s">
+        <v>379</v>
+      </c>
+      <c r="AM1" s="12" t="s">
+        <v>380</v>
+      </c>
+      <c r="AN1" s="12" t="s">
+        <v>381</v>
+      </c>
+      <c r="AO1" s="12" t="s">
+        <v>382</v>
+      </c>
+      <c r="AP1" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="AQ1" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="AH1" s="15" t="s">
+      <c r="AR1" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="AI1" s="15" t="s">
+      <c r="AS1" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="AJ1" s="15" t="s">
+      <c r="AT1" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="AK1" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="AL1" s="15" t="s">
+      <c r="AU1" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="AM1" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="AN1" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="AO1" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="AP1" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AQ1" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR1" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="AS1" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="AT1" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="AU1" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="AV1" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="AW1" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="AX1" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="AY1" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="AZ1" s="17" t="s">
-        <v>68</v>
+      <c r="AV1" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="AW1" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="AX1" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="AY1" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ1" s="14" t="s">
+        <v>57</v>
       </c>
       <c r="BA1" s="5" t="s">
         <v>0</v>
@@ -4731,194 +4900,195 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:58" s="38" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="O2" s="84" t="s">
+        <v>125</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="U2" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="V2" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="W2" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="X2" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="7" t="s">
+      <c r="Y2" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="J2" s="7" t="s">
+      <c r="Z2" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA2" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB2" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="AC2" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="AD2" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="M2" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="O2" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="P2" s="18" t="s">
+      <c r="AE2" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF2" s="85" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG2" s="86" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH2" s="86" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI2" s="86" t="s">
+        <v>384</v>
+      </c>
+      <c r="AJ2" s="86" t="s">
         <v>102</v>
       </c>
-      <c r="Q2" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="S2" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="T2" s="7" t="s">
+      <c r="AK2" s="86" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL2" s="86" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM2" s="86" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN2" s="86" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO2" s="86" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP2" s="86" t="s">
         <v>103</v>
       </c>
-      <c r="U2" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="V2" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="W2" s="7" t="s">
+      <c r="AQ2" s="87" t="s">
+        <v>59</v>
+      </c>
+      <c r="AR2" s="87" t="s">
+        <v>129</v>
+      </c>
+      <c r="AS2" s="87" t="s">
+        <v>60</v>
+      </c>
+      <c r="AT2" s="87" t="s">
+        <v>61</v>
+      </c>
+      <c r="AU2" s="87" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV2" s="88" t="s">
+        <v>59</v>
+      </c>
+      <c r="AW2" s="88" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX2" s="88" t="s">
+        <v>60</v>
+      </c>
+      <c r="AY2" s="88" t="s">
+        <v>61</v>
+      </c>
+      <c r="AZ2" s="88" t="s">
+        <v>62</v>
+      </c>
+      <c r="BA2" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="BB2" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="BC2" s="89" t="s">
+        <v>7</v>
+      </c>
+      <c r="BD2" s="88" t="s">
+        <v>5</v>
+      </c>
+      <c r="BE2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="BF2" s="88" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:58" s="17" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="X2" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="Y2" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z2" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="AA2" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AB2" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="AC2" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="AD2" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="AE2" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="AF2" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="AG2" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="AH2" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="AI2" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="AJ2" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="AK2" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL2" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="AM2" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="AN2" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="AO2" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP2" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="AQ2" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AR2" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="AS2" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="AT2" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="AU2" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="AV2" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="AW2" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="AX2" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="AY2" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="AZ2" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="BA2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="BB2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="BC2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="BD2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="BE2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="BF2" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:58" s="20" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="M3" s="21"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
+      <c r="M3" s="18"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="25"/>
+      <c r="AF3" s="64"/>
     </row>
     <row r="4" spans="1:58" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>34</v>
@@ -4927,9 +5097,9 @@
         <v>35</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E4" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -4954,58 +5124,58 @@
         <v>41</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="N4" s="8">
+        <v>123</v>
+      </c>
+      <c r="N4" s="7">
         <v>390</v>
       </c>
-      <c r="O4" s="8">
+      <c r="O4" s="7">
         <v>50.22</v>
       </c>
-      <c r="P4" s="18" t="s">
+      <c r="P4" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="Q4" s="9" t="s">
+      <c r="Q4" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="R4" s="18" t="s">
+      <c r="R4" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="S4" s="18" t="s">
-        <v>132</v>
+      <c r="S4" s="15" t="s">
+        <v>120</v>
       </c>
       <c r="U4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AQ4" s="16">
+      <c r="AQ4" s="13">
         <v>1</v>
       </c>
-      <c r="AR4" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="AS4" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="AT4" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="AU4" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="AV4" s="10">
+      <c r="AR4" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="AS4" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT4" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="AU4" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="AV4" s="9">
         <v>2</v>
       </c>
-      <c r="AW4" s="10">
+      <c r="AW4" s="9">
         <v>1</v>
       </c>
-      <c r="AX4" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="AY4" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="AZ4" s="10" t="s">
-        <v>78</v>
+      <c r="AX4" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AY4" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="AZ4" s="9" t="s">
+        <v>67</v>
       </c>
       <c r="BA4" s="3" t="s">
         <v>45</v>
@@ -5013,61 +5183,61 @@
       <c r="BB4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="BD4" s="11" t="s">
+      <c r="BD4" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="BE4" s="10" t="s">
+      <c r="BE4" s="9" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="Q1 BB1:BC1 A1:M1 BG1:XFD1">
-    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="25" priority="24" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1">
-    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="24" priority="22" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",P1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:S1">
-    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="23" priority="21" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",R1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE1:BF1">
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",BE1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1">
-    <cfRule type="expression" dxfId="11" priority="9">
+    <cfRule type="expression" dxfId="21" priority="15">
       <formula>IF(COUNTIF($S$4:$S$1048576,"*"&amp;LEFT(T$1, FIND(".", T$1)-1)&amp;"*"),"FALSE","TRUE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1">
-    <cfRule type="expression" dxfId="10" priority="5">
+    <cfRule type="expression" dxfId="20" priority="11">
       <formula>IF(COUNTIF($S$4:$S$1048576,"*"&amp;LEFT(T$1, FIND(".", T$1)-1)&amp;"*"),"TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:AD1">
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="19" priority="9">
       <formula>IF(COUNTIF($S$4:$S$1048576,"*"&amp;LEFT(U$1, FIND(".", U$1)-1)&amp;"*"),"FALSE","TRUE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:AD1">
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="18" priority="10">
       <formula>IF(COUNTIF($S$4:$S$1048576,"*"&amp;LEFT(U$1, FIND(".", U$1)-1)&amp;"*"),"TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:O1">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="17" priority="7">
       <formula>IF(COUNTIF($M$4:$M$1048576,"*"&amp;LEFT(N$1, FIND(".", N$1)-1)&amp;"*"),"FALSE","TRUE")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:O1">
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="16" priority="8">
       <formula>IF(COUNTIF($M$4:$M$1048576,"*"&amp;LEFT(N$1, FIND(".", N$1)-1)&amp;"*"),"TRUE","FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5093,20 +5263,20 @@
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="6" max="8" width="15.5703125" customWidth="1"/>
     <col min="9" max="9" width="26.140625" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" style="39" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" style="34" customWidth="1"/>
     <col min="11" max="12" width="8.7109375" style="2" customWidth="1"/>
     <col min="13" max="15" width="8.7109375" customWidth="1"/>
-    <col min="16" max="17" width="15.5703125" style="67" customWidth="1"/>
+    <col min="16" max="17" width="15.5703125" style="55" customWidth="1"/>
     <col min="18" max="19" width="15.5703125" customWidth="1"/>
-    <col min="20" max="21" width="15.5703125" style="67" customWidth="1"/>
-    <col min="22" max="28" width="8.7109375" style="78" customWidth="1"/>
-    <col min="29" max="29" width="9.140625" style="78"/>
+    <col min="20" max="21" width="15.5703125" style="55" customWidth="1"/>
+    <col min="22" max="28" width="8.7109375" style="65" customWidth="1"/>
+    <col min="29" max="29" width="9.140625" style="65"/>
     <col min="30" max="36" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>347</v>
+        <v>318</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -5115,24 +5285,24 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>348</v>
+        <v>319</v>
       </c>
       <c r="E1" t="s">
-        <v>349</v>
+        <v>320</v>
       </c>
       <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="82" t="s">
-        <v>350</v>
-      </c>
-      <c r="H1" s="51" t="s">
-        <v>189</v>
-      </c>
-      <c r="I1" s="51" t="s">
-        <v>190</v>
-      </c>
-      <c r="J1" s="35" t="s">
+      <c r="G1" s="69" t="s">
+        <v>321</v>
+      </c>
+      <c r="H1" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="I1" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="J1" s="31" t="s">
         <v>0</v>
       </c>
       <c r="K1" s="4" t="s">
@@ -5150,195 +5320,195 @@
       <c r="O1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="53" t="s">
-        <v>209</v>
-      </c>
-      <c r="Q1" s="53" t="s">
-        <v>210</v>
-      </c>
-      <c r="R1" s="53" t="s">
-        <v>209</v>
-      </c>
-      <c r="S1" s="53" t="s">
-        <v>210</v>
-      </c>
-      <c r="T1" s="53" t="s">
-        <v>209</v>
-      </c>
-      <c r="U1" s="53" t="s">
-        <v>210</v>
-      </c>
-      <c r="V1" s="54" t="s">
-        <v>211</v>
-      </c>
-      <c r="W1" s="54" t="s">
-        <v>212</v>
-      </c>
-      <c r="X1" s="54" t="s">
-        <v>213</v>
-      </c>
-      <c r="Y1" s="54" t="s">
-        <v>214</v>
-      </c>
-      <c r="Z1" s="54" t="s">
-        <v>215</v>
-      </c>
-      <c r="AA1" s="54" t="s">
-        <v>351</v>
-      </c>
-      <c r="AB1" s="54" t="s">
-        <v>352</v>
-      </c>
-      <c r="AC1" s="54" t="s">
-        <v>353</v>
-      </c>
-      <c r="AD1" s="54" t="s">
-        <v>211</v>
-      </c>
-      <c r="AE1" s="54" t="s">
-        <v>212</v>
-      </c>
-      <c r="AF1" s="54" t="s">
-        <v>213</v>
-      </c>
-      <c r="AG1" s="54" t="s">
-        <v>214</v>
-      </c>
-      <c r="AH1" s="54" t="s">
-        <v>215</v>
-      </c>
-      <c r="AI1" s="54" t="s">
-        <v>351</v>
-      </c>
-      <c r="AJ1" s="54" t="s">
-        <v>352</v>
-      </c>
-      <c r="AK1" s="54" t="s">
-        <v>353</v>
+      <c r="P1" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q1" s="46" t="s">
+        <v>198</v>
+      </c>
+      <c r="R1" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="S1" s="46" t="s">
+        <v>198</v>
+      </c>
+      <c r="T1" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="U1" s="46" t="s">
+        <v>198</v>
+      </c>
+      <c r="V1" s="47" t="s">
+        <v>199</v>
+      </c>
+      <c r="W1" s="47" t="s">
+        <v>200</v>
+      </c>
+      <c r="X1" s="47" t="s">
+        <v>201</v>
+      </c>
+      <c r="Y1" s="47" t="s">
+        <v>202</v>
+      </c>
+      <c r="Z1" s="47" t="s">
+        <v>203</v>
+      </c>
+      <c r="AA1" s="47" t="s">
+        <v>322</v>
+      </c>
+      <c r="AB1" s="47" t="s">
+        <v>323</v>
+      </c>
+      <c r="AC1" s="47" t="s">
+        <v>324</v>
+      </c>
+      <c r="AD1" s="47" t="s">
+        <v>199</v>
+      </c>
+      <c r="AE1" s="47" t="s">
+        <v>200</v>
+      </c>
+      <c r="AF1" s="47" t="s">
+        <v>201</v>
+      </c>
+      <c r="AG1" s="47" t="s">
+        <v>202</v>
+      </c>
+      <c r="AH1" s="47" t="s">
+        <v>203</v>
+      </c>
+      <c r="AI1" s="47" t="s">
+        <v>322</v>
+      </c>
+      <c r="AJ1" s="47" t="s">
+        <v>323</v>
+      </c>
+      <c r="AK1" s="47" t="s">
+        <v>324</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>354</v>
-      </c>
-      <c r="B2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" t="s">
-        <v>355</v>
-      </c>
-      <c r="E2" s="37" t="s">
-        <v>356</v>
-      </c>
-      <c r="F2" t="s">
-        <v>357</v>
-      </c>
-      <c r="G2" s="38" t="s">
-        <v>358</v>
-      </c>
-      <c r="H2" s="38" t="s">
-        <v>359</v>
-      </c>
-      <c r="I2" s="38" t="s">
-        <v>360</v>
+    <row r="2" spans="1:37" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>325</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>326</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>327</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>328</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>329</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>330</v>
+      </c>
+      <c r="I2" s="33" t="s">
+        <v>331</v>
       </c>
       <c r="J2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="60" t="s">
-        <v>361</v>
-      </c>
-      <c r="Q2" s="60" t="s">
-        <v>362</v>
-      </c>
-      <c r="R2" s="38" t="s">
-        <v>361</v>
-      </c>
-      <c r="S2" s="38" t="s">
-        <v>362</v>
-      </c>
-      <c r="T2" s="60" t="s">
-        <v>361</v>
-      </c>
-      <c r="U2" s="60" t="s">
-        <v>362</v>
-      </c>
-      <c r="V2" s="77" t="s">
-        <v>363</v>
-      </c>
-      <c r="W2" s="77" t="s">
-        <v>364</v>
-      </c>
-      <c r="X2" s="78" t="s">
-        <v>255</v>
-      </c>
-      <c r="Y2" s="78" t="s">
-        <v>256</v>
-      </c>
-      <c r="Z2" s="78" t="s">
-        <v>257</v>
-      </c>
-      <c r="AA2" s="78" t="s">
-        <v>365</v>
-      </c>
-      <c r="AB2" s="78" t="s">
-        <v>366</v>
-      </c>
-      <c r="AC2" s="78" t="s">
-        <v>367</v>
-      </c>
-      <c r="AD2" s="38" t="s">
-        <v>363</v>
-      </c>
-      <c r="AE2" s="38" t="s">
-        <v>364</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>255</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>256</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>257</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>365</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>368</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>367</v>
+      <c r="P2" s="77" t="s">
+        <v>332</v>
+      </c>
+      <c r="Q2" s="77" t="s">
+        <v>333</v>
+      </c>
+      <c r="R2" s="33" t="s">
+        <v>332</v>
+      </c>
+      <c r="S2" s="33" t="s">
+        <v>333</v>
+      </c>
+      <c r="T2" s="77" t="s">
+        <v>332</v>
+      </c>
+      <c r="U2" s="77" t="s">
+        <v>333</v>
+      </c>
+      <c r="V2" s="90" t="s">
+        <v>334</v>
+      </c>
+      <c r="W2" s="90" t="s">
+        <v>335</v>
+      </c>
+      <c r="X2" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="Y2" s="91" t="s">
+        <v>227</v>
+      </c>
+      <c r="Z2" s="91" t="s">
+        <v>228</v>
+      </c>
+      <c r="AA2" s="91" t="s">
+        <v>336</v>
+      </c>
+      <c r="AB2" s="91" t="s">
+        <v>337</v>
+      </c>
+      <c r="AC2" s="91" t="s">
+        <v>338</v>
+      </c>
+      <c r="AD2" s="33" t="s">
+        <v>334</v>
+      </c>
+      <c r="AE2" s="33" t="s">
+        <v>335</v>
+      </c>
+      <c r="AF2" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="AG2" s="38" t="s">
+        <v>227</v>
+      </c>
+      <c r="AH2" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="AI2" s="38" t="s">
+        <v>336</v>
+      </c>
+      <c r="AJ2" s="38" t="s">
+        <v>339</v>
+      </c>
+      <c r="AK2" s="38" t="s">
+        <v>338</v>
       </c>
     </row>
-    <row r="3" spans="1:37" s="80" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="79" t="s">
-        <v>118</v>
-      </c>
-      <c r="M3" s="81"/>
+    <row r="3" spans="1:37" s="67" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="66" t="s">
+        <v>106</v>
+      </c>
+      <c r="M3" s="68"/>
     </row>
     <row r="4" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>369</v>
+        <v>340</v>
       </c>
       <c r="B4" t="s">
         <v>43</v>
@@ -5347,130 +5517,130 @@
         <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>370</v>
+        <v>341</v>
       </c>
       <c r="E4" t="s">
         <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>371</v>
+        <v>342</v>
       </c>
       <c r="G4" t="s">
-        <v>372</v>
+        <v>343</v>
       </c>
       <c r="H4" t="s">
-        <v>272</v>
+        <v>243</v>
       </c>
       <c r="I4" t="s">
-        <v>273</v>
-      </c>
-      <c r="J4" s="39" t="s">
-        <v>373</v>
+        <v>244</v>
+      </c>
+      <c r="J4" s="34" t="s">
+        <v>344</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>374</v>
+        <v>345</v>
       </c>
       <c r="M4" t="s">
-        <v>375</v>
+        <v>346</v>
       </c>
       <c r="N4" t="s">
-        <v>376</v>
-      </c>
-      <c r="P4" s="67" t="s">
-        <v>291</v>
-      </c>
-      <c r="Q4" s="67" t="s">
-        <v>292</v>
+        <v>347</v>
+      </c>
+      <c r="P4" s="55" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q4" s="55" t="s">
+        <v>263</v>
       </c>
       <c r="R4" t="s">
-        <v>293</v>
+        <v>264</v>
       </c>
       <c r="S4" t="s">
-        <v>294</v>
-      </c>
-      <c r="T4" s="67" t="s">
-        <v>295</v>
-      </c>
-      <c r="U4" s="67" t="s">
-        <v>296</v>
-      </c>
-      <c r="V4" s="78" t="s">
-        <v>377</v>
-      </c>
-      <c r="W4" s="78" t="s">
-        <v>298</v>
-      </c>
-      <c r="X4" s="78" t="s">
-        <v>255</v>
-      </c>
-      <c r="Y4" s="78" t="s">
-        <v>303</v>
-      </c>
-      <c r="Z4" s="78" t="s">
-        <v>304</v>
-      </c>
-      <c r="AA4" s="78" t="s">
-        <v>378</v>
-      </c>
-      <c r="AB4" s="78" t="s">
-        <v>379</v>
-      </c>
-      <c r="AC4" s="78" t="s">
-        <v>380</v>
+        <v>265</v>
+      </c>
+      <c r="T4" s="55" t="s">
+        <v>266</v>
+      </c>
+      <c r="U4" s="55" t="s">
+        <v>267</v>
+      </c>
+      <c r="V4" s="65" t="s">
+        <v>348</v>
+      </c>
+      <c r="W4" s="65" t="s">
+        <v>269</v>
+      </c>
+      <c r="X4" s="65" t="s">
+        <v>226</v>
+      </c>
+      <c r="Y4" s="65" t="s">
+        <v>274</v>
+      </c>
+      <c r="Z4" s="65" t="s">
+        <v>275</v>
+      </c>
+      <c r="AA4" s="65" t="s">
+        <v>349</v>
+      </c>
+      <c r="AB4" s="65" t="s">
+        <v>350</v>
+      </c>
+      <c r="AC4" s="65" t="s">
+        <v>351</v>
       </c>
       <c r="AD4" t="s">
-        <v>381</v>
+        <v>352</v>
       </c>
       <c r="AE4" t="s">
-        <v>382</v>
+        <v>353</v>
       </c>
       <c r="AF4" t="s">
-        <v>255</v>
+        <v>226</v>
       </c>
       <c r="AG4" t="s">
-        <v>383</v>
+        <v>354</v>
       </c>
       <c r="AH4" t="s">
-        <v>384</v>
+        <v>355</v>
       </c>
       <c r="AI4" t="s">
-        <v>378</v>
+        <v>349</v>
       </c>
       <c r="AJ4" t="s">
-        <v>379</v>
+        <v>350</v>
       </c>
       <c r="AK4" t="s">
-        <v>380</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:G1 K1:L1 V1:AC1 AL1:XFD1 P1:Q1">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:S1">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",R1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:U1">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",T1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:I1">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD1:AK1">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",AD1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:O1">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="~*">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="~*">
       <formula>NOT(ISERROR(SEARCH("~*",N1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>